<commit_message>
change backend and correct times
</commit_message>
<xml_diff>
--- a/timesv5.xlsx
+++ b/timesv5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian Leprevost\Documents\SemLink\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\install\SemLink\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBF7B37-9196-4FA1-BB5B-B106A2A23ED1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1DABCF-A647-448D-9C3E-95428BE62FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-114" yWindow="-114" windowWidth="23254" windowHeight="13174" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRE1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <sheet name="INF1" sheetId="7" r:id="rId5"/>
     <sheet name="INF2" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="25">
   <si>
     <t>block</t>
   </si>
@@ -100,9 +111,6 @@
   </si>
   <si>
     <t>(difference = time at the end where opensesame runs alone, so time for fMRI to turn off and on)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -597,48 +605,48 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -654,7 +662,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -950,18 +958,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -984,7 +992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -1022,7 +1030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -1060,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1.68</v>
       </c>
@@ -1098,7 +1106,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1.96</v>
       </c>
@@ -1136,7 +1144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>1.96</v>
       </c>
@@ -1174,7 +1182,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1.68</v>
       </c>
@@ -1212,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>2.8</v>
       </c>
@@ -1250,7 +1258,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1.96</v>
       </c>
@@ -1288,7 +1296,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1.68</v>
       </c>
@@ -1326,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>3.08</v>
       </c>
@@ -1364,7 +1372,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>9.24</v>
       </c>
@@ -1402,7 +1410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>1.68</v>
       </c>
@@ -1440,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>1.96</v>
       </c>
@@ -1478,7 +1486,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2.52</v>
       </c>
@@ -1516,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>1.68</v>
       </c>
@@ -1554,7 +1562,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>1.68</v>
       </c>
@@ -1592,7 +1600,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>1.96</v>
       </c>
@@ -1630,7 +1638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>2.52</v>
       </c>
@@ -1668,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>1.68</v>
       </c>
@@ -1706,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>3.92</v>
       </c>
@@ -1744,7 +1752,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>1.68</v>
       </c>
@@ -1782,30 +1790,30 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L23">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1813,36 +1821,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
       <c r="B25">
         <f>SUM(B3:C24)</f>
-        <v>86.920000000000016</v>
+        <v>84.920000000000016</v>
       </c>
       <c r="D25">
         <f>SUM(D3:E24)</f>
-        <v>83.839999999999989</v>
+        <v>81.839999999999989</v>
       </c>
       <c r="F25">
         <f>SUM(F3:G24)</f>
-        <v>85.84</v>
+        <v>83.84</v>
       </c>
       <c r="H25">
         <f>SUM(H3:I24)</f>
-        <v>84.56</v>
+        <v>82.56</v>
       </c>
       <c r="J25">
         <f>SUM(J3:K24)</f>
-        <v>84.24</v>
+        <v>82.24</v>
       </c>
       <c r="L25">
         <f>SUM(L3:M24)</f>
-        <v>86.120000000000019</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>84.120000000000019</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1850,7 +1858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1858,7 +1866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1887,7 +1895,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1911,109 +1919,110 @@
         <f>1*2.8</f>
         <v>2.8</v>
       </c>
-      <c r="L31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <f>1*2.8</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
       <c r="B33">
         <f>B31+B29+B25</f>
-        <v>155.32000000000002</v>
+        <v>153.32000000000002</v>
       </c>
       <c r="D33">
         <f>D31+D29+D25</f>
-        <v>146.63999999999999</v>
+        <v>144.63999999999999</v>
       </c>
       <c r="F33">
         <f>F31+F29+F25</f>
-        <v>148.63999999999999</v>
+        <v>146.63999999999999</v>
       </c>
       <c r="H33">
         <f>H31+H29+H25</f>
-        <v>147.36000000000001</v>
+        <v>145.36000000000001</v>
       </c>
       <c r="J33">
         <f>J31+J29+J25</f>
-        <v>147.04</v>
-      </c>
-      <c r="L33" t="e">
+        <v>145.04</v>
+      </c>
+      <c r="L33">
         <f>L31+L29+L25</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <v>146.92000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>16</v>
       </c>
       <c r="B34">
         <f>B33-2</f>
-        <v>153.32000000000002</v>
+        <v>151.32000000000002</v>
       </c>
       <c r="D34">
         <f>D33-2</f>
-        <v>144.63999999999999</v>
+        <v>142.63999999999999</v>
       </c>
       <c r="F34">
         <f>F33-2</f>
-        <v>146.63999999999999</v>
+        <v>144.63999999999999</v>
       </c>
       <c r="H34">
         <f>H33-2</f>
-        <v>145.36000000000001</v>
+        <v>143.36000000000001</v>
       </c>
       <c r="J34">
         <f>J33-2</f>
-        <v>145.04</v>
-      </c>
-      <c r="L34" t="e">
+        <v>143.04</v>
+      </c>
+      <c r="L34">
         <f>L33-2</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>144.92000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B35">
         <f>B34/2.8</f>
-        <v>54.757142857142867</v>
+        <v>54.042857142857152</v>
       </c>
       <c r="D35">
         <f t="shared" ref="D35:L35" si="0">D34/2.8</f>
-        <v>51.657142857142858</v>
+        <v>50.942857142857143</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>52.371428571428567</v>
+        <v>51.657142857142858</v>
       </c>
       <c r="H35">
         <f t="shared" si="0"/>
-        <v>51.914285714285725</v>
+        <v>51.20000000000001</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>51.8</v>
-      </c>
-      <c r="L35" t="e">
+        <v>51.085714285714289</v>
+      </c>
+      <c r="L35">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>51.757142857142867</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B36" s="1">
         <f>ROUND(B35,0)</f>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1">
         <f>ROUND(D35,0)</f>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1">
@@ -2023,35 +2032,35 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1">
         <f>ROUND(H35,0)</f>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1">
         <f>ROUND(J35,0)</f>
+        <v>51</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1">
+        <f>ROUND(L35,0)</f>
         <v>52</v>
       </c>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1" t="e">
-        <f>ROUND(L35,0)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>17</v>
       </c>
       <c r="B38">
         <f>B36*2.8</f>
-        <v>154</v>
+        <v>151.19999999999999</v>
       </c>
       <c r="D38">
         <f>D36*2.8</f>
-        <v>145.6</v>
+        <v>142.79999999999998</v>
       </c>
       <c r="F38">
         <f>F36*2.8</f>
@@ -2059,114 +2068,124 @@
       </c>
       <c r="H38">
         <f>H36*2.8</f>
-        <v>145.6</v>
+        <v>142.79999999999998</v>
       </c>
       <c r="J38">
         <f>J36*2.8</f>
+        <v>142.79999999999998</v>
+      </c>
+      <c r="L38">
+        <f>L36*2.8</f>
         <v>145.6</v>
       </c>
-      <c r="L38" t="e">
-        <f>L36*2.8</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N38" s="1" t="e">
+      <c r="N38" s="1">
         <f>(SUM(B38:L38))/60</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <v>14.513333333333332</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>18</v>
       </c>
       <c r="B39">
         <f>B31+B29+B25</f>
-        <v>155.32000000000002</v>
+        <v>153.32000000000002</v>
       </c>
       <c r="D39">
         <f>D31+D29+D25</f>
-        <v>146.63999999999999</v>
+        <v>144.63999999999999</v>
       </c>
       <c r="F39">
         <f>F31+F29+F25</f>
-        <v>148.63999999999999</v>
+        <v>146.63999999999999</v>
       </c>
       <c r="H39">
         <f>H31+H29+H25</f>
-        <v>147.36000000000001</v>
+        <v>145.36000000000001</v>
       </c>
       <c r="J39">
         <f>J31+J29+J25</f>
-        <v>147.04</v>
-      </c>
-      <c r="L39" t="e">
+        <v>145.04</v>
+      </c>
+      <c r="L39">
         <f>L31+L29+L25</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N39" s="1" t="e">
+        <v>146.92000000000002</v>
+      </c>
+      <c r="N39" s="1">
         <f>(SUM(B39:L39))/60</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+        <v>14.698666666666668</v>
+      </c>
+      <c r="O39">
+        <v>14</v>
+      </c>
+      <c r="P39">
+        <v>5</v>
+      </c>
+      <c r="Q39" s="1">
+        <f>N39+(O39*P39)/60</f>
+        <v>15.865333333333334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>20</v>
       </c>
       <c r="B40">
         <f>B39-B38</f>
-        <v>1.3200000000000216</v>
+        <v>2.120000000000033</v>
       </c>
       <c r="D40">
         <f>D39-D38</f>
-        <v>1.039999999999992</v>
+        <v>1.8400000000000034</v>
       </c>
       <c r="F40">
         <f>F39-F38</f>
-        <v>3.039999999999992</v>
+        <v>1.039999999999992</v>
       </c>
       <c r="H40">
         <f>H39-H38</f>
-        <v>1.7600000000000193</v>
+        <v>2.5600000000000307</v>
       </c>
       <c r="J40">
         <f>J39-J38</f>
-        <v>1.4399999999999977</v>
-      </c>
-      <c r="L40" t="e">
+        <v>2.2400000000000091</v>
+      </c>
+      <c r="L40">
         <f>L39-L38</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.3200000000000216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>12</v>
       </c>
@@ -2178,18 +2197,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2212,7 +2231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2250,7 +2269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -2288,7 +2307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1.68</v>
       </c>
@@ -2326,7 +2345,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2.2400000000000002</v>
       </c>
@@ -2364,7 +2383,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>1.4</v>
       </c>
@@ -2402,7 +2421,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>2.2400000000000002</v>
       </c>
@@ -2440,7 +2459,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1.68</v>
       </c>
@@ -2478,7 +2497,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1.4</v>
       </c>
@@ -2516,7 +2535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1.68</v>
       </c>
@@ -2554,7 +2573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>3.08</v>
       </c>
@@ -2592,7 +2611,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>2.2400000000000002</v>
       </c>
@@ -2630,7 +2649,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>7.84</v>
       </c>
@@ -2668,7 +2687,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2.8</v>
       </c>
@@ -2706,7 +2725,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>4.4800000000000004</v>
       </c>
@@ -2744,7 +2763,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>1.68</v>
       </c>
@@ -2782,7 +2801,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>3.36</v>
       </c>
@@ -2820,7 +2839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>1.68</v>
       </c>
@@ -2858,7 +2877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>1.68</v>
       </c>
@@ -2896,7 +2915,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>1.68</v>
       </c>
@@ -2934,7 +2953,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>1.68</v>
       </c>
@@ -2972,7 +2991,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>2.52</v>
       </c>
@@ -3010,30 +3029,30 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L23">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -3041,36 +3060,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
       <c r="B25">
         <f>SUM(B3:C24)</f>
-        <v>85.84</v>
+        <v>83.84</v>
       </c>
       <c r="D25">
         <f>SUM(D3:E24)</f>
-        <v>83.279999999999987</v>
+        <v>81.279999999999987</v>
       </c>
       <c r="F25">
         <f>SUM(F3:G24)</f>
-        <v>85.04</v>
+        <v>83.04</v>
       </c>
       <c r="H25">
         <f>SUM(H3:I24)</f>
-        <v>85.64</v>
+        <v>83.64</v>
       </c>
       <c r="J25">
         <f>SUM(J3:K24)</f>
-        <v>85.760000000000019</v>
+        <v>83.760000000000019</v>
       </c>
       <c r="L25">
         <f>SUM(L3:M24)</f>
-        <v>85.11999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>83.11999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -3078,7 +3097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -3086,7 +3105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -3115,7 +3134,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -3144,94 +3163,94 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
       <c r="B33">
         <f>B31+B29+B25</f>
-        <v>154.24</v>
+        <v>152.24</v>
       </c>
       <c r="D33">
         <f>D31+D29+D25</f>
-        <v>146.07999999999998</v>
+        <v>144.07999999999998</v>
       </c>
       <c r="F33">
         <f>F31+F29+F25</f>
-        <v>147.84</v>
+        <v>145.84</v>
       </c>
       <c r="H33">
         <f>H31+H29+H25</f>
-        <v>148.44</v>
+        <v>146.44</v>
       </c>
       <c r="J33">
         <f>J31+J29+J25</f>
-        <v>148.56</v>
+        <v>146.56</v>
       </c>
       <c r="L33">
         <f>L31+L29+L25</f>
-        <v>147.91999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <v>145.91999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>16</v>
       </c>
       <c r="B34">
         <f>B33-2</f>
-        <v>152.24</v>
+        <v>150.24</v>
       </c>
       <c r="D34">
         <f>D33-2</f>
-        <v>144.07999999999998</v>
+        <v>142.07999999999998</v>
       </c>
       <c r="F34">
         <f>F33-2</f>
-        <v>145.84</v>
+        <v>143.84</v>
       </c>
       <c r="H34">
         <f>H33-2</f>
-        <v>146.44</v>
+        <v>144.44</v>
       </c>
       <c r="J34">
         <f>J33-2</f>
-        <v>146.56</v>
+        <v>144.56</v>
       </c>
       <c r="L34">
         <f>L33-2</f>
-        <v>145.91999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>143.91999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B35">
         <f>B34/2.8</f>
-        <v>54.371428571428581</v>
+        <v>53.657142857142865</v>
       </c>
       <c r="D35">
         <f t="shared" ref="D35:L35" si="0">D34/2.8</f>
-        <v>51.457142857142856</v>
+        <v>50.74285714285714</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>52.085714285714289</v>
+        <v>51.371428571428574</v>
       </c>
       <c r="H35">
         <f t="shared" si="0"/>
-        <v>52.300000000000004</v>
+        <v>51.585714285714289</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>52.342857142857149</v>
+        <v>51.628571428571433</v>
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
-        <v>52.114285714285714</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
@@ -3247,7 +3266,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1">
         <f>ROUND(F35,0)</f>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1">
@@ -3262,15 +3281,15 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1">
         <f>ROUND(L35,0)</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -3284,7 +3303,7 @@
       </c>
       <c r="F38">
         <f>F36*2.8</f>
-        <v>145.6</v>
+        <v>142.79999999999998</v>
       </c>
       <c r="H38">
         <f>H36*2.8</f>
@@ -3296,106 +3315,116 @@
       </c>
       <c r="L38">
         <f>L36*2.8</f>
-        <v>145.6</v>
+        <v>142.79999999999998</v>
       </c>
       <c r="N38" s="1">
         <f>(SUM(B38:L38))/60</f>
-        <v>14.606666666666667</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <v>14.513333333333332</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>18</v>
       </c>
       <c r="B39">
         <f>B31+B29+B25</f>
-        <v>154.24</v>
+        <v>152.24</v>
       </c>
       <c r="D39">
         <f>D31+D29+D25</f>
-        <v>146.07999999999998</v>
+        <v>144.07999999999998</v>
       </c>
       <c r="F39">
         <f>F31+F29+F25</f>
-        <v>147.84</v>
+        <v>145.84</v>
       </c>
       <c r="H39">
         <f>H31+H29+H25</f>
-        <v>148.44</v>
+        <v>146.44</v>
       </c>
       <c r="J39">
         <f>J31+J29+J25</f>
-        <v>148.56</v>
+        <v>146.56</v>
       </c>
       <c r="L39">
         <f>L31+L29+L25</f>
-        <v>147.91999999999999</v>
+        <v>145.91999999999999</v>
       </c>
       <c r="N39" s="1">
         <f>(SUM(B39:L39))/60</f>
-        <v>14.884666666666664</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+        <v>14.684666666666663</v>
+      </c>
+      <c r="O39">
+        <v>14</v>
+      </c>
+      <c r="P39">
+        <v>5</v>
+      </c>
+      <c r="Q39" s="1">
+        <f>N39+(O39*P39)/60</f>
+        <v>15.851333333333329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>20</v>
       </c>
       <c r="B40">
         <f>B39-B38</f>
-        <v>3.0400000000000205</v>
+        <v>1.0400000000000205</v>
       </c>
       <c r="D40">
         <f>D39-D38</f>
-        <v>3.2800000000000011</v>
+        <v>1.2800000000000011</v>
       </c>
       <c r="F40">
         <f>F39-F38</f>
-        <v>2.2400000000000091</v>
+        <v>3.0400000000000205</v>
       </c>
       <c r="H40">
         <f>H39-H38</f>
-        <v>2.8400000000000034</v>
+        <v>0.84000000000000341</v>
       </c>
       <c r="J40">
         <f>J39-J38</f>
-        <v>2.960000000000008</v>
+        <v>0.96000000000000796</v>
       </c>
       <c r="L40">
         <f>L39-L38</f>
-        <v>2.3199999999999932</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3.1200000000000045</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>12</v>
       </c>
@@ -3407,18 +3436,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+      <selection activeCell="Q68" sqref="Q68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3435,7 +3464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -3461,7 +3490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -3487,7 +3516,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2.2400000000000002</v>
       </c>
@@ -3513,7 +3542,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>6.16</v>
       </c>
@@ -3539,7 +3568,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>1.1200000000000001</v>
       </c>
@@ -3565,7 +3594,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>0.84</v>
       </c>
@@ -3591,7 +3620,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1.1200000000000001</v>
       </c>
@@ -3617,7 +3646,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2.2400000000000002</v>
       </c>
@@ -3643,7 +3672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>0.84</v>
       </c>
@@ -3669,7 +3698,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>0.56000000000000005</v>
       </c>
@@ -3695,7 +3724,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0.84</v>
       </c>
@@ -3721,7 +3750,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>2.52</v>
       </c>
@@ -3747,7 +3776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>0.56000000000000005</v>
       </c>
@@ -3773,7 +3802,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1.68</v>
       </c>
@@ -3799,7 +3828,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0.56000000000000005</v>
       </c>
@@ -3825,7 +3854,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0.84</v>
       </c>
@@ -3851,7 +3880,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>3.92</v>
       </c>
@@ -3877,7 +3906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>0.84</v>
       </c>
@@ -3903,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>0.56000000000000005</v>
       </c>
@@ -3929,7 +3958,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>2.2400000000000002</v>
       </c>
@@ -3955,7 +3984,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>3.92</v>
       </c>
@@ -3981,7 +4010,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>1.68</v>
       </c>
@@ -4007,7 +4036,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>2.52</v>
       </c>
@@ -4033,7 +4062,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>3.64</v>
       </c>
@@ -4059,7 +4088,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>3.08</v>
       </c>
@@ -4085,7 +4114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>0.56000000000000005</v>
       </c>
@@ -4111,7 +4140,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>8.68</v>
       </c>
@@ -4137,7 +4166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>0.84</v>
       </c>
@@ -4163,7 +4192,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>0.84</v>
       </c>
@@ -4189,7 +4218,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>0.84</v>
       </c>
@@ -4215,7 +4244,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>1.1200000000000001</v>
       </c>
@@ -4241,7 +4270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>1.1200000000000001</v>
       </c>
@@ -4267,7 +4296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>3.36</v>
       </c>
@@ -4293,7 +4322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>0.84</v>
       </c>
@@ -4319,7 +4348,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>0.84</v>
       </c>
@@ -4345,7 +4374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>8.1199999999999992</v>
       </c>
@@ -4371,7 +4400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>2.2400000000000002</v>
       </c>
@@ -4397,7 +4426,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>0.84</v>
       </c>
@@ -4423,7 +4452,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>1.96</v>
       </c>
@@ -4449,7 +4478,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>0.84</v>
       </c>
@@ -4475,7 +4504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>1.1200000000000001</v>
       </c>
@@ -4501,7 +4530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>2.52</v>
       </c>
@@ -4527,7 +4556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>0.84</v>
       </c>
@@ -4553,7 +4582,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>0.84</v>
       </c>
@@ -4579,7 +4608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>0.84</v>
       </c>
@@ -4605,7 +4634,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>1.1200000000000001</v>
       </c>
@@ -4631,7 +4660,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>0.84</v>
       </c>
@@ -4657,7 +4686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>5.04</v>
       </c>
@@ -4683,7 +4712,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>1.1200000000000001</v>
       </c>
@@ -4709,24 +4738,24 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>4</v>
       </c>
       <c r="B52">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D52">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F52">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H52">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -4734,28 +4763,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>6</v>
       </c>
       <c r="B54">
         <f>SUM(B3:C53)</f>
-        <v>158.84000000000006</v>
+        <v>156.84000000000006</v>
       </c>
       <c r="D54">
         <f>SUM(D3:E53)</f>
-        <v>156.16000000000008</v>
+        <v>154.16000000000008</v>
       </c>
       <c r="F54">
         <f>SUM(F3:G53)</f>
-        <v>146.08000000000004</v>
+        <v>144.08000000000004</v>
       </c>
       <c r="H54">
         <f>SUM(H3:I53)</f>
-        <v>157.28000000000003</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>155.28000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>23</v>
       </c>
@@ -4763,7 +4792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -4771,7 +4800,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>22</v>
       </c>
@@ -4792,7 +4821,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -4813,70 +4842,70 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>19</v>
       </c>
       <c r="B62">
         <f>B60+B58+B54</f>
-        <v>311.24000000000007</v>
+        <v>309.24000000000007</v>
       </c>
       <c r="D62">
         <f>D60+D58+D54</f>
-        <v>302.96000000000009</v>
+        <v>300.96000000000009</v>
       </c>
       <c r="F62">
         <f>F60+F58+F54</f>
-        <v>292.88000000000005</v>
+        <v>290.88000000000005</v>
       </c>
       <c r="H62">
         <f>H60+H58+H54</f>
-        <v>304.08000000000004</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>302.08000000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>16</v>
       </c>
       <c r="B63">
         <f>B62-2</f>
-        <v>309.24000000000007</v>
+        <v>307.24000000000007</v>
       </c>
       <c r="D63">
         <f>D62-2</f>
-        <v>300.96000000000009</v>
+        <v>298.96000000000009</v>
       </c>
       <c r="F63">
         <f>F62-2</f>
-        <v>290.88000000000005</v>
+        <v>288.88000000000005</v>
       </c>
       <c r="H63">
         <f>H62-2</f>
-        <v>302.08000000000004</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>300.08000000000004</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B64">
         <f>B63/2.8</f>
-        <v>110.44285714285718</v>
+        <v>109.72857142857146</v>
       </c>
       <c r="D64">
         <f t="shared" ref="D64:H64" si="0">D63/2.8</f>
-        <v>107.48571428571432</v>
+        <v>106.77142857142861</v>
       </c>
       <c r="F64">
         <f t="shared" si="0"/>
-        <v>103.88571428571431</v>
+        <v>103.17142857142859</v>
       </c>
       <c r="H64">
         <f t="shared" si="0"/>
-        <v>107.8857142857143</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+        <v>107.17142857142859</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>15</v>
       </c>
@@ -4892,24 +4921,24 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1">
         <f>ROUND(F64,0)</f>
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1">
         <f>ROUND(H64,0)</f>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N66" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -4923,79 +4952,89 @@
       </c>
       <c r="F67">
         <f>F65*2.8</f>
-        <v>291.2</v>
+        <v>288.39999999999998</v>
       </c>
       <c r="H67">
         <f>H65*2.8</f>
-        <v>302.39999999999998</v>
+        <v>299.59999999999997</v>
       </c>
       <c r="N67" s="1">
         <f>(SUM(B67:L67))/60</f>
-        <v>20.019999999999996</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+        <v>19.926666666666666</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>18</v>
       </c>
       <c r="B68">
         <f>B60+B58+B54</f>
-        <v>311.24000000000007</v>
+        <v>309.24000000000007</v>
       </c>
       <c r="D68">
         <f>D60+D58+D54</f>
-        <v>302.96000000000009</v>
+        <v>300.96000000000009</v>
       </c>
       <c r="F68">
         <f>F60+F58+F54</f>
-        <v>292.88000000000005</v>
+        <v>290.88000000000005</v>
       </c>
       <c r="H68">
         <f>H60+H58+H54</f>
-        <v>304.08000000000004</v>
+        <v>302.08000000000004</v>
       </c>
       <c r="N68" s="1">
         <f>(SUM(B68:L68))/60</f>
-        <v>20.186000000000003</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+        <v>20.052666666666671</v>
+      </c>
+      <c r="O68">
+        <v>14</v>
+      </c>
+      <c r="P68">
+        <v>3</v>
+      </c>
+      <c r="Q68" s="1">
+        <f>N68+(O68*P68)/60</f>
+        <v>20.75266666666667</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>20</v>
       </c>
       <c r="B69">
         <f>B68-B67</f>
-        <v>3.2400000000000659</v>
+        <v>1.2400000000000659</v>
       </c>
       <c r="D69">
         <f>D68-D67</f>
-        <v>3.3600000000001273</v>
+        <v>1.3600000000001273</v>
       </c>
       <c r="F69">
         <f>F68-F67</f>
-        <v>1.6800000000000637</v>
+        <v>2.480000000000075</v>
       </c>
       <c r="H69">
         <f>H68-H67</f>
-        <v>1.6800000000000637</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2.480000000000075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>9</v>
       </c>
@@ -5007,18 +5046,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+      <selection activeCell="Q68" sqref="O68:Q68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5035,7 +5074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -5061,7 +5100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -5087,7 +5126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1.4</v>
       </c>
@@ -5113,7 +5152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1.68</v>
       </c>
@@ -5139,7 +5178,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0.84</v>
       </c>
@@ -5165,7 +5204,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>2.52</v>
       </c>
@@ -5191,7 +5230,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>0.84</v>
       </c>
@@ -5217,7 +5256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1.4</v>
       </c>
@@ -5243,7 +5282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1.68</v>
       </c>
@@ -5269,7 +5308,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>3.92</v>
       </c>
@@ -5295,7 +5334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0.84</v>
       </c>
@@ -5321,7 +5360,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0.84</v>
       </c>
@@ -5347,7 +5386,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>0.56000000000000005</v>
       </c>
@@ -5373,7 +5412,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1.96</v>
       </c>
@@ -5399,7 +5438,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0.84</v>
       </c>
@@ -5425,7 +5464,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>2.8</v>
       </c>
@@ -5451,7 +5490,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>3.36</v>
       </c>
@@ -5477,7 +5516,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>3.08</v>
       </c>
@@ -5503,7 +5542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>0.56000000000000005</v>
       </c>
@@ -5529,7 +5568,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>1.96</v>
       </c>
@@ -5555,7 +5594,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>1.96</v>
       </c>
@@ -5581,7 +5620,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>1.96</v>
       </c>
@@ -5607,7 +5646,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>1.1200000000000001</v>
       </c>
@@ -5633,7 +5672,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>1.1200000000000001</v>
       </c>
@@ -5659,7 +5698,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>3.92</v>
       </c>
@@ -5685,7 +5724,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>3.64</v>
       </c>
@@ -5711,7 +5750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>1.68</v>
       </c>
@@ -5737,7 +5776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>2.2400000000000002</v>
       </c>
@@ -5763,7 +5802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>0.56000000000000005</v>
       </c>
@@ -5789,7 +5828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>5.88</v>
       </c>
@@ -5815,7 +5854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>1.68</v>
       </c>
@@ -5841,7 +5880,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>1.4</v>
       </c>
@@ -5867,7 +5906,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>1.4</v>
       </c>
@@ -5893,7 +5932,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>0.84</v>
       </c>
@@ -5919,7 +5958,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>1.1200000000000001</v>
       </c>
@@ -5945,7 +5984,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>1.1200000000000001</v>
       </c>
@@ -5971,7 +6010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>1.1200000000000001</v>
       </c>
@@ -5997,7 +6036,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>5.88</v>
       </c>
@@ -6023,7 +6062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>1.4</v>
       </c>
@@ -6049,7 +6088,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>0.84</v>
       </c>
@@ -6075,7 +6114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>1.4</v>
       </c>
@@ -6101,7 +6140,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>0.84</v>
       </c>
@@ -6127,7 +6166,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>1.68</v>
       </c>
@@ -6153,7 +6192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>2.2400000000000002</v>
       </c>
@@ -6179,7 +6218,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>0.56000000000000005</v>
       </c>
@@ -6205,7 +6244,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>3.08</v>
       </c>
@@ -6231,7 +6270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>1.68</v>
       </c>
@@ -6257,7 +6296,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>0.56000000000000005</v>
       </c>
@@ -6283,7 +6322,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>1.1200000000000001</v>
       </c>
@@ -6309,24 +6348,24 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>4</v>
       </c>
       <c r="B52">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D52">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F52">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H52">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -6334,28 +6373,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>6</v>
       </c>
       <c r="B54">
         <f>SUM(B3:C53)</f>
-        <v>152.12000000000003</v>
+        <v>150.12000000000003</v>
       </c>
       <c r="D54">
         <f>SUM(D3:E53)</f>
-        <v>156.44000000000005</v>
+        <v>154.44000000000005</v>
       </c>
       <c r="F54">
         <f>SUM(F3:G53)</f>
-        <v>143.84000000000003</v>
+        <v>141.84000000000003</v>
       </c>
       <c r="H54">
         <f>SUM(H3:I53)</f>
-        <v>156.44000000000008</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>154.44000000000008</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>23</v>
       </c>
@@ -6363,7 +6402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -6371,7 +6410,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>22</v>
       </c>
@@ -6392,7 +6431,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -6413,189 +6452,199 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>19</v>
       </c>
       <c r="B62">
         <f>B60+B58+B54</f>
-        <v>304.52000000000004</v>
+        <v>302.52000000000004</v>
       </c>
       <c r="D62">
         <f>D60+D58+D54</f>
-        <v>303.24000000000007</v>
+        <v>301.24000000000007</v>
       </c>
       <c r="F62">
         <f>F60+F58+F54</f>
-        <v>290.64000000000004</v>
+        <v>288.64000000000004</v>
       </c>
       <c r="H62">
         <f>H60+H58+H54</f>
-        <v>303.24000000000012</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>301.24000000000012</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>16</v>
       </c>
       <c r="B63">
         <f>B62-2</f>
-        <v>302.52000000000004</v>
+        <v>300.52000000000004</v>
       </c>
       <c r="D63">
         <f>D62-2</f>
-        <v>301.24000000000007</v>
+        <v>299.24000000000007</v>
       </c>
       <c r="F63">
         <f>F62-2</f>
-        <v>288.64000000000004</v>
+        <v>286.64000000000004</v>
       </c>
       <c r="H63">
         <f>H62-2</f>
-        <v>301.24000000000012</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>299.24000000000012</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B64">
         <f>B63/2.8</f>
-        <v>108.04285714285716</v>
+        <v>107.32857142857145</v>
       </c>
       <c r="D64">
         <f t="shared" ref="D64:H64" si="0">D63/2.8</f>
-        <v>107.58571428571432</v>
+        <v>106.87142857142859</v>
       </c>
       <c r="F64">
         <f t="shared" si="0"/>
-        <v>103.0857142857143</v>
+        <v>102.37142857142859</v>
       </c>
       <c r="H64">
         <f t="shared" si="0"/>
-        <v>107.58571428571433</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+        <v>106.87142857142862</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B65" s="1">
         <f>ROUND(B64,0)</f>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1">
         <f>ROUND(D64,0)</f>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1">
         <f>ROUND(F64,0)</f>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1">
         <f>ROUND(H64,0)</f>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N66" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>17</v>
       </c>
       <c r="B67">
         <f>B65*2.8</f>
-        <v>302.39999999999998</v>
+        <v>299.59999999999997</v>
       </c>
       <c r="D67">
         <f>D65*2.8</f>
-        <v>302.39999999999998</v>
+        <v>299.59999999999997</v>
       </c>
       <c r="F67">
         <f>F65*2.8</f>
-        <v>288.39999999999998</v>
+        <v>285.59999999999997</v>
       </c>
       <c r="H67">
         <f>H65*2.8</f>
-        <v>302.39999999999998</v>
+        <v>299.59999999999997</v>
       </c>
       <c r="N67" s="1">
         <f>(SUM(B67:L67))/60</f>
-        <v>19.926666666666666</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+        <v>19.739999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>18</v>
       </c>
       <c r="B68">
         <f>B60+B58+B54</f>
-        <v>304.52000000000004</v>
+        <v>302.52000000000004</v>
       </c>
       <c r="D68">
         <f>D60+D58+D54</f>
-        <v>303.24000000000007</v>
+        <v>301.24000000000007</v>
       </c>
       <c r="F68">
         <f>F60+F58+F54</f>
-        <v>290.64000000000004</v>
+        <v>288.64000000000004</v>
       </c>
       <c r="H68">
         <f>H60+H58+H54</f>
-        <v>303.24000000000012</v>
+        <v>301.24000000000012</v>
       </c>
       <c r="N68" s="1">
         <f>(SUM(B68:L68))/60</f>
-        <v>20.027333333333338</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+        <v>19.894000000000005</v>
+      </c>
+      <c r="O68">
+        <v>14</v>
+      </c>
+      <c r="P68">
+        <v>3</v>
+      </c>
+      <c r="Q68" s="1">
+        <f>N68+(O68*P68)/60</f>
+        <v>20.594000000000005</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>20</v>
       </c>
       <c r="B69">
         <f>B68-B67</f>
-        <v>2.1200000000000614</v>
+        <v>2.9200000000000728</v>
       </c>
       <c r="D69">
         <f>D68-D67</f>
-        <v>0.84000000000008868</v>
+        <v>1.6400000000001</v>
       </c>
       <c r="F69">
         <f>F68-F67</f>
-        <v>2.2400000000000659</v>
+        <v>3.0400000000000773</v>
       </c>
       <c r="H69">
         <f>H68-H67</f>
-        <v>0.84000000000014552</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.6400000000001569</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>9</v>
       </c>
@@ -6607,18 +6656,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="Q52" sqref="O52:Q52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6635,7 +6684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -6661,7 +6710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -6687,7 +6736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0.56000000000000005</v>
       </c>
@@ -6713,7 +6762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2.52</v>
       </c>
@@ -6739,7 +6788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>1.4</v>
       </c>
@@ -6765,7 +6814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1.96</v>
       </c>
@@ -6791,7 +6840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1.1200000000000001</v>
       </c>
@@ -6817,7 +6866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1.68</v>
       </c>
@@ -6843,7 +6892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1.1200000000000001</v>
       </c>
@@ -6869,7 +6918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1.4</v>
       </c>
@@ -6895,7 +6944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1.4</v>
       </c>
@@ -6921,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>1.96</v>
       </c>
@@ -6947,7 +6996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>0.56000000000000005</v>
       </c>
@@ -6973,7 +7022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2.8</v>
       </c>
@@ -6999,7 +7048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>3.64</v>
       </c>
@@ -7025,7 +7074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0.56000000000000005</v>
       </c>
@@ -7051,7 +7100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>1.1200000000000001</v>
       </c>
@@ -7077,7 +7126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>2.52</v>
       </c>
@@ -7103,7 +7152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>0.84</v>
       </c>
@@ -7129,7 +7178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>0.84</v>
       </c>
@@ -7155,7 +7204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>1.68</v>
       </c>
@@ -7181,7 +7230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>0.56000000000000005</v>
       </c>
@@ -7207,7 +7256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>0.56000000000000005</v>
       </c>
@@ -7233,7 +7282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>1.68</v>
       </c>
@@ -7259,7 +7308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>0.84</v>
       </c>
@@ -7285,7 +7334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>3.08</v>
       </c>
@@ -7311,7 +7360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>1.96</v>
       </c>
@@ -7337,7 +7386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>4.76</v>
       </c>
@@ -7363,7 +7412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>2.2400000000000002</v>
       </c>
@@ -7389,7 +7438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>1.68</v>
       </c>
@@ -7415,7 +7464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>0.84</v>
       </c>
@@ -7441,7 +7490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>0.84</v>
       </c>
@@ -7467,7 +7516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>1.4</v>
       </c>
@@ -7493,24 +7542,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="B36">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F36">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H36">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -7518,28 +7567,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>6</v>
       </c>
       <c r="B38">
         <f>SUM(B3:C37)</f>
-        <v>101.12000000000003</v>
+        <v>99.120000000000033</v>
       </c>
       <c r="D38">
         <f>SUM(D3:E37)</f>
-        <v>109.64000000000003</v>
+        <v>107.64000000000003</v>
       </c>
       <c r="F38">
         <f>SUM(F3:G37)</f>
-        <v>111.32000000000001</v>
+        <v>109.32000000000001</v>
       </c>
       <c r="H38">
         <f>SUM(H3:I37)</f>
-        <v>110.48000000000005</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>108.48000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -7547,7 +7596,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -7555,7 +7604,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -7576,7 +7625,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -7597,189 +7646,199 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>19</v>
       </c>
       <c r="B46">
         <f>B44+B42+B38</f>
-        <v>157.52000000000004</v>
+        <v>155.52000000000004</v>
       </c>
       <c r="D46">
         <f>D44+D42+D38</f>
-        <v>160.44000000000003</v>
+        <v>158.44000000000003</v>
       </c>
       <c r="F46">
         <f>F44+F42+F38</f>
-        <v>162.12</v>
+        <v>160.12</v>
       </c>
       <c r="H46">
         <f>H44+H42+H38</f>
-        <v>161.28000000000003</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159.28000000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>16</v>
       </c>
       <c r="B47">
         <f>B46-2</f>
-        <v>155.52000000000004</v>
+        <v>153.52000000000004</v>
       </c>
       <c r="D47">
         <f>D46-2</f>
-        <v>158.44000000000003</v>
+        <v>156.44000000000003</v>
       </c>
       <c r="F47">
         <f>F46-2</f>
-        <v>160.12</v>
+        <v>158.12</v>
       </c>
       <c r="H47">
         <f>H46-2</f>
-        <v>159.28000000000003</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>157.28000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B48">
         <f>B47/2.8</f>
-        <v>55.542857142857159</v>
+        <v>54.828571428571443</v>
       </c>
       <c r="D48">
         <f t="shared" ref="D48:H48" si="0">D47/2.8</f>
-        <v>56.585714285714296</v>
+        <v>55.871428571428581</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
-        <v>57.18571428571429</v>
+        <v>56.471428571428575</v>
       </c>
       <c r="H48">
         <f t="shared" si="0"/>
-        <v>56.8857142857143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+        <v>56.171428571428585</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B49" s="1">
         <f>ROUND(B48,0)</f>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1">
         <f>ROUND(D48,0)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1">
         <f>ROUND(F48,0)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1">
         <f>ROUND(H48,0)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N50" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>17</v>
       </c>
       <c r="B51">
         <f>B49*2.8</f>
-        <v>156.79999999999998</v>
+        <v>154</v>
       </c>
       <c r="D51">
         <f>D49*2.8</f>
-        <v>159.6</v>
+        <v>156.79999999999998</v>
       </c>
       <c r="F51">
         <f>F49*2.8</f>
-        <v>159.6</v>
+        <v>156.79999999999998</v>
       </c>
       <c r="H51">
         <f>H49*2.8</f>
-        <v>159.6</v>
+        <v>156.79999999999998</v>
       </c>
       <c r="N51" s="1">
         <f>(SUM(B51:L51))/60</f>
-        <v>10.593333333333334</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10.406666666666665</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>18</v>
       </c>
       <c r="B52">
         <f>B44+B42+B38</f>
-        <v>157.52000000000004</v>
+        <v>155.52000000000004</v>
       </c>
       <c r="D52">
         <f>D44+D42+D38</f>
-        <v>160.44000000000003</v>
+        <v>158.44000000000003</v>
       </c>
       <c r="F52">
         <f>F44+F42+F38</f>
-        <v>162.12</v>
+        <v>160.12</v>
       </c>
       <c r="H52">
         <f>H44+H42+H38</f>
-        <v>161.28000000000003</v>
+        <v>159.28000000000003</v>
       </c>
       <c r="N52" s="1">
         <f>(SUM(B52:L52))/60</f>
-        <v>10.689333333333336</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10.556000000000003</v>
+      </c>
+      <c r="O52">
+        <v>14</v>
+      </c>
+      <c r="P52">
+        <v>3</v>
+      </c>
+      <c r="Q52" s="1">
+        <f>N52+(O52*P52)/60</f>
+        <v>11.256000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>20</v>
       </c>
       <c r="B53">
         <f>B52-B51</f>
-        <v>0.72000000000005571</v>
+        <v>1.5200000000000387</v>
       </c>
       <c r="D53">
         <f>D52-D51</f>
-        <v>0.84000000000003183</v>
+        <v>1.6400000000000432</v>
       </c>
       <c r="F53">
         <f>F52-F51</f>
-        <v>2.5200000000000102</v>
+        <v>3.3200000000000216</v>
       </c>
       <c r="H53">
         <f>H52-H51</f>
-        <v>1.6800000000000352</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2.4800000000000466</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>9</v>
       </c>
@@ -7791,18 +7850,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7819,7 +7878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -7845,7 +7904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -7871,7 +7930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0.84</v>
       </c>
@@ -7897,7 +7956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>0.84</v>
       </c>
@@ -7923,7 +7982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>7.28</v>
       </c>
@@ -7949,7 +8008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>2.52</v>
       </c>
@@ -7975,7 +8034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1.1200000000000001</v>
       </c>
@@ -8001,7 +8060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1.96</v>
       </c>
@@ -8027,7 +8086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>0.84</v>
       </c>
@@ -8053,7 +8112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>0.84</v>
       </c>
@@ -8079,7 +8138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0.84</v>
       </c>
@@ -8105,7 +8164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0.56000000000000005</v>
       </c>
@@ -8131,7 +8190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>1.68</v>
       </c>
@@ -8157,7 +8216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1.68</v>
       </c>
@@ -8183,7 +8242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0.84</v>
       </c>
@@ -8209,7 +8268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0.84</v>
       </c>
@@ -8235,7 +8294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>1.68</v>
       </c>
@@ -8261,7 +8320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>0.84</v>
       </c>
@@ -8287,7 +8346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>0.56000000000000005</v>
       </c>
@@ -8313,7 +8372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>0.84</v>
       </c>
@@ -8339,7 +8398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>0.84</v>
       </c>
@@ -8365,7 +8424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>6.72</v>
       </c>
@@ -8391,7 +8450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>5.88</v>
       </c>
@@ -8417,7 +8476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>1.1200000000000001</v>
       </c>
@@ -8443,7 +8502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>1.1200000000000001</v>
       </c>
@@ -8469,7 +8528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>1.1200000000000001</v>
       </c>
@@ -8495,7 +8554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>4.76</v>
       </c>
@@ -8521,7 +8580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>1.68</v>
       </c>
@@ -8547,7 +8606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>3.36</v>
       </c>
@@ -8573,7 +8632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>3.92</v>
       </c>
@@ -8599,7 +8658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>0.84</v>
       </c>
@@ -8625,7 +8684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>1.1200000000000001</v>
       </c>
@@ -8651,7 +8710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>0.56000000000000005</v>
       </c>
@@ -8677,24 +8736,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="B36">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F36">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H36">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -8702,28 +8761,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>6</v>
       </c>
       <c r="B38">
         <f>SUM(B3:C37)</f>
-        <v>110.64000000000006</v>
+        <v>108.64000000000006</v>
       </c>
       <c r="D38">
         <f>SUM(D3:E37)</f>
-        <v>107.12000000000003</v>
+        <v>105.12000000000003</v>
       </c>
       <c r="F38">
         <f>SUM(F3:G37)</f>
-        <v>110.76000000000003</v>
+        <v>108.76000000000003</v>
       </c>
       <c r="H38">
         <f>SUM(H3:I37)</f>
-        <v>101.24000000000004</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>99.240000000000038</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -8731,7 +8790,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -8739,7 +8798,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -8760,7 +8819,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -8781,189 +8840,199 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>19</v>
       </c>
       <c r="B46">
         <f>B44+B42+B38</f>
-        <v>167.04000000000005</v>
+        <v>165.04000000000005</v>
       </c>
       <c r="D46">
         <f>D44+D42+D38</f>
-        <v>157.92000000000002</v>
+        <v>155.92000000000002</v>
       </c>
       <c r="F46">
         <f>F44+F42+F38</f>
-        <v>161.56000000000003</v>
+        <v>159.56000000000003</v>
       </c>
       <c r="H46">
         <f>H44+H42+H38</f>
-        <v>152.04000000000002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>150.04000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>16</v>
       </c>
       <c r="B47">
         <f>B46-2</f>
-        <v>165.04000000000005</v>
+        <v>163.04000000000005</v>
       </c>
       <c r="D47">
         <f>D46-2</f>
-        <v>155.92000000000002</v>
+        <v>153.92000000000002</v>
       </c>
       <c r="F47">
         <f>F46-2</f>
-        <v>159.56000000000003</v>
+        <v>157.56000000000003</v>
       </c>
       <c r="H47">
         <f>H46-2</f>
-        <v>150.04000000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>148.04000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B48">
         <f>B47/2.8</f>
-        <v>58.942857142857164</v>
+        <v>58.228571428571449</v>
       </c>
       <c r="D48">
         <f t="shared" ref="D48:H48" si="0">D47/2.8</f>
-        <v>55.685714285714297</v>
+        <v>54.971428571428582</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
-        <v>56.985714285714302</v>
+        <v>56.271428571428586</v>
       </c>
       <c r="H48">
         <f t="shared" si="0"/>
-        <v>53.585714285714296</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+        <v>52.871428571428581</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B49" s="1">
         <f>ROUND(B48,0)</f>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1">
         <f>ROUND(D48,0)</f>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1">
         <f>ROUND(F48,0)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1">
         <f>ROUND(H48,0)</f>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N50" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>17</v>
       </c>
       <c r="B51">
         <f>B49*2.8</f>
-        <v>165.2</v>
+        <v>162.39999999999998</v>
       </c>
       <c r="D51">
         <f>D49*2.8</f>
-        <v>156.79999999999998</v>
+        <v>154</v>
       </c>
       <c r="F51">
         <f>F49*2.8</f>
-        <v>159.6</v>
+        <v>156.79999999999998</v>
       </c>
       <c r="H51">
         <f>H49*2.8</f>
-        <v>151.19999999999999</v>
+        <v>148.39999999999998</v>
       </c>
       <c r="N51" s="1">
         <f>(SUM(B51:L51))/60</f>
-        <v>10.546666666666665</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10.359999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>18</v>
       </c>
       <c r="B52">
         <f>B44+B42+B38</f>
-        <v>167.04000000000005</v>
+        <v>165.04000000000005</v>
       </c>
       <c r="D52">
         <f>D44+D42+D38</f>
-        <v>157.92000000000002</v>
+        <v>155.92000000000002</v>
       </c>
       <c r="F52">
         <f>F44+F42+F38</f>
-        <v>161.56000000000003</v>
+        <v>159.56000000000003</v>
       </c>
       <c r="H52">
         <f>H44+H42+H38</f>
-        <v>152.04000000000002</v>
+        <v>150.04000000000002</v>
       </c>
       <c r="N52" s="1">
         <f>(SUM(B52:L52))/60</f>
-        <v>10.642666666666669</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10.509333333333336</v>
+      </c>
+      <c r="O52">
+        <v>14</v>
+      </c>
+      <c r="P52">
+        <v>3</v>
+      </c>
+      <c r="Q52" s="1">
+        <f>N52+(O52*P52)/60</f>
+        <v>11.209333333333335</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>20</v>
       </c>
       <c r="B53">
         <f>B52-B51</f>
-        <v>1.8400000000000603</v>
+        <v>2.6400000000000716</v>
       </c>
       <c r="D53">
         <f>D52-D51</f>
-        <v>1.120000000000033</v>
+        <v>1.9200000000000159</v>
       </c>
       <c r="F53">
         <f>F52-F51</f>
-        <v>1.9600000000000364</v>
+        <v>2.7600000000000477</v>
       </c>
       <c r="H53">
         <f>H52-H51</f>
-        <v>0.84000000000003183</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.6400000000000432</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
fix times, pariticpant list
</commit_message>
<xml_diff>
--- a/timesv5.xlsx
+++ b/timesv5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\install\SemLink\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian Leprevost\Documents\SemLink\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1DABCF-A647-448D-9C3E-95428BE62FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5583B27-34F0-419D-AA4F-7F70D27738CC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-114" yWindow="-114" windowWidth="23254" windowHeight="13174" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRE1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <sheet name="INF1" sheetId="7" r:id="rId5"/>
     <sheet name="INF2" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="24">
   <si>
     <t>block</t>
   </si>
@@ -59,22 +48,10 @@
     <t>total ISI ITI</t>
   </si>
   <si>
-    <t>3 vol before each block</t>
-  </si>
-  <si>
     <t>what is best 1) opensesame finish first, continue loop, start again thinking it is a new run</t>
   </si>
   <si>
     <t>potential problem = run spend too much time before opensesame start, so stop scanning too early</t>
-  </si>
-  <si>
-    <t>I need to know time it takes to "relaunch a run"</t>
-  </si>
-  <si>
-    <t>let's assume it is 3s for simplicity</t>
-  </si>
-  <si>
-    <t>difference = time open sesame runs alone = good</t>
   </si>
   <si>
     <t>2) opensesame finish last, the second run already started =&gt; solution opensesame 2s&gt;</t>
@@ -86,13 +63,7 @@
     <t>round</t>
   </si>
   <si>
-    <t>remove 2s so finish 1st</t>
-  </si>
-  <si>
     <t>run time</t>
-  </si>
-  <si>
-    <t>opensesame time</t>
   </si>
   <si>
     <t>total duration</t>
@@ -111,6 +82,21 @@
   </si>
   <si>
     <t>(difference = time at the end where opensesame runs alone, so time for fMRI to turn off and on)</t>
+  </si>
+  <si>
+    <t>opensesame time (+7s)</t>
+  </si>
+  <si>
+    <t>times between runs = between 13 and 14 seconds =&gt; add 7 s to opensesame to be in between</t>
+  </si>
+  <si>
+    <t>(remaining interrun time)</t>
+  </si>
+  <si>
+    <t>3/1 vol before each block</t>
+  </si>
+  <si>
+    <t>difference (in s)</t>
   </si>
 </sst>
 </file>
@@ -600,53 +586,54 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -662,7 +649,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -958,18 +945,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -992,7 +979,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -1030,7 +1017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -1068,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1.68</v>
       </c>
@@ -1106,7 +1093,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1.96</v>
       </c>
@@ -1144,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.96</v>
       </c>
@@ -1182,7 +1169,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1.68</v>
       </c>
@@ -1220,7 +1207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2.8</v>
       </c>
@@ -1258,7 +1245,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1.96</v>
       </c>
@@ -1296,7 +1283,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1.68</v>
       </c>
@@ -1334,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>3.08</v>
       </c>
@@ -1372,7 +1359,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9.24</v>
       </c>
@@ -1410,7 +1397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1.68</v>
       </c>
@@ -1448,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1.96</v>
       </c>
@@ -1486,7 +1473,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2.52</v>
       </c>
@@ -1524,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1.68</v>
       </c>
@@ -1562,7 +1549,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>1.68</v>
       </c>
@@ -1600,7 +1587,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1.96</v>
       </c>
@@ -1638,7 +1625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2.52</v>
       </c>
@@ -1676,7 +1663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>1.68</v>
       </c>
@@ -1714,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>3.92</v>
       </c>
@@ -1752,7 +1739,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>1.68</v>
       </c>
@@ -1790,7 +1777,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1813,7 +1800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1821,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1850,15 +1837,15 @@
         <v>84.120000000000019</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1866,9 +1853,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B29">
         <f>B28*B27</f>
@@ -1895,9 +1882,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B31">
         <f>3*2.8</f>
@@ -1915,18 +1902,10 @@
         <f>1*2.8</f>
         <v>2.8</v>
       </c>
-      <c r="J31">
-        <f>1*2.8</f>
-        <v>2.8</v>
-      </c>
-      <c r="L31">
-        <f>1*2.8</f>
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B33">
         <f>B31+B29+B25</f>
@@ -1946,248 +1925,192 @@
       </c>
       <c r="J33">
         <f>J31+J29+J25</f>
-        <v>145.04</v>
+        <v>142.24</v>
       </c>
       <c r="L33">
         <f>L31+L29+L25</f>
-        <v>146.92000000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>16</v>
+        <v>144.12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B34">
-        <f>B33-2</f>
-        <v>151.32000000000002</v>
+        <f>B33/2.8</f>
+        <v>54.757142857142867</v>
       </c>
       <c r="D34">
-        <f>D33-2</f>
-        <v>142.63999999999999</v>
+        <f>D33/2.8</f>
+        <v>51.657142857142858</v>
       </c>
       <c r="F34">
-        <f>F33-2</f>
-        <v>144.63999999999999</v>
+        <f>F33/2.8</f>
+        <v>52.371428571428567</v>
       </c>
       <c r="H34">
-        <f>H33-2</f>
-        <v>143.36000000000001</v>
+        <f>H33/2.8</f>
+        <v>51.914285714285725</v>
       </c>
       <c r="J34">
-        <f>J33-2</f>
-        <v>143.04</v>
+        <f>J33/2.8</f>
+        <v>50.800000000000004</v>
       </c>
       <c r="L34">
-        <f>L33-2</f>
-        <v>144.92000000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+        <f>L33/2.8</f>
+        <v>51.471428571428575</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35">
-        <f>B34/2.8</f>
-        <v>54.042857142857152</v>
-      </c>
-      <c r="D35">
-        <f t="shared" ref="D35:L35" si="0">D34/2.8</f>
-        <v>50.942857142857143</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="0"/>
-        <v>51.657142857142858</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="0"/>
-        <v>51.20000000000001</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="0"/>
-        <v>51.085714285714289</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="0"/>
-        <v>51.757142857142867</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="1">
+        <f>ROUND(B34,0)</f>
+        <v>55</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1">
+        <f>ROUND(D34,0)</f>
+        <v>52</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1">
+        <f>ROUND(F34,0)</f>
+        <v>52</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1">
+        <f>ROUND(H34,0)</f>
+        <v>52</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1">
+        <f>ROUND(J34,0)</f>
+        <v>51</v>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1">
+        <f>ROUND(L34,0)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R36" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="1">
-        <f>ROUND(B35,0)</f>
-        <v>54</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1">
-        <f>ROUND(D35,0)</f>
-        <v>51</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1">
-        <f>ROUND(F35,0)</f>
-        <v>52</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1">
-        <f>ROUND(H35,0)</f>
-        <v>51</v>
-      </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1">
-        <f>ROUND(J35,0)</f>
-        <v>51</v>
-      </c>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1">
-        <f>ROUND(L35,0)</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N37" t="s">
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <f>B35*2.8</f>
+        <v>154</v>
+      </c>
+      <c r="D37">
+        <f>D35*2.8</f>
+        <v>145.6</v>
+      </c>
+      <c r="F37">
+        <f>F35*2.8</f>
+        <v>145.6</v>
+      </c>
+      <c r="H37">
+        <f>H35*2.8</f>
+        <v>145.6</v>
+      </c>
+      <c r="J37">
+        <f>J35*2.8</f>
+        <v>142.79999999999998</v>
+      </c>
+      <c r="L37">
+        <f>L35*2.8</f>
+        <v>142.79999999999998</v>
+      </c>
+      <c r="R37" s="2">
+        <f>(SUM(B37:L37))/60</f>
+        <v>14.606666666666666</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38">
+        <f>B33+7</f>
+        <v>160.32000000000002</v>
+      </c>
+      <c r="D38">
+        <f>D33+7</f>
+        <v>151.63999999999999</v>
+      </c>
+      <c r="F38">
+        <f>F33+7</f>
+        <v>153.63999999999999</v>
+      </c>
+      <c r="H38">
+        <f>H33+7</f>
+        <v>152.36000000000001</v>
+      </c>
+      <c r="J38">
+        <f>J33+7</f>
+        <v>149.24</v>
+      </c>
+      <c r="L38">
+        <f>L33+7</f>
+        <v>151.12</v>
+      </c>
+      <c r="R38" s="2">
+        <f>(SUM(B38:L38))/60</f>
+        <v>15.305333333333333</v>
+      </c>
+      <c r="S38">
+        <v>7</v>
+      </c>
+      <c r="T38">
+        <v>3</v>
+      </c>
+      <c r="U38" s="1">
+        <f>R38+T38*S38/60</f>
+        <v>15.655333333333333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39">
+        <f>B38-B37</f>
+        <v>6.3200000000000216</v>
+      </c>
+      <c r="D39">
+        <f>D38-D37</f>
+        <v>6.039999999999992</v>
+      </c>
+      <c r="F39">
+        <f>F38-F37</f>
+        <v>8.039999999999992</v>
+      </c>
+      <c r="H39">
+        <f>H38-H37</f>
+        <v>6.7600000000000193</v>
+      </c>
+      <c r="J39">
+        <f>J38-J37</f>
+        <v>6.4400000000000261</v>
+      </c>
+      <c r="L39">
+        <f>L38-L37</f>
+        <v>8.3200000000000216</v>
+      </c>
+      <c r="S39" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38">
-        <f>B36*2.8</f>
-        <v>151.19999999999999</v>
-      </c>
-      <c r="D38">
-        <f>D36*2.8</f>
-        <v>142.79999999999998</v>
-      </c>
-      <c r="F38">
-        <f>F36*2.8</f>
-        <v>145.6</v>
-      </c>
-      <c r="H38">
-        <f>H36*2.8</f>
-        <v>142.79999999999998</v>
-      </c>
-      <c r="J38">
-        <f>J36*2.8</f>
-        <v>142.79999999999998</v>
-      </c>
-      <c r="L38">
-        <f>L36*2.8</f>
-        <v>145.6</v>
-      </c>
-      <c r="N38" s="1">
-        <f>(SUM(B38:L38))/60</f>
-        <v>14.513333333333332</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>18</v>
-      </c>
-      <c r="B39">
-        <f>B31+B29+B25</f>
-        <v>153.32000000000002</v>
-      </c>
-      <c r="D39">
-        <f>D31+D29+D25</f>
-        <v>144.63999999999999</v>
-      </c>
-      <c r="F39">
-        <f>F31+F29+F25</f>
-        <v>146.63999999999999</v>
-      </c>
-      <c r="H39">
-        <f>H31+H29+H25</f>
-        <v>145.36000000000001</v>
-      </c>
-      <c r="J39">
-        <f>J31+J29+J25</f>
-        <v>145.04</v>
-      </c>
-      <c r="L39">
-        <f>L31+L29+L25</f>
-        <v>146.92000000000002</v>
-      </c>
-      <c r="N39" s="1">
-        <f>(SUM(B39:L39))/60</f>
-        <v>14.698666666666668</v>
-      </c>
-      <c r="O39">
-        <v>14</v>
-      </c>
-      <c r="P39">
-        <v>5</v>
-      </c>
-      <c r="Q39" s="1">
-        <f>N39+(O39*P39)/60</f>
-        <v>15.865333333333334</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40">
-        <f>B39-B38</f>
-        <v>2.120000000000033</v>
-      </c>
-      <c r="D40">
-        <f>D39-D38</f>
-        <v>1.8400000000000034</v>
-      </c>
-      <c r="F40">
-        <f>F39-F38</f>
-        <v>1.039999999999992</v>
-      </c>
-      <c r="H40">
-        <f>H39-H38</f>
-        <v>2.5600000000000307</v>
-      </c>
-      <c r="J40">
-        <f>J39-J38</f>
-        <v>2.2400000000000091</v>
-      </c>
-      <c r="L40">
-        <f>L39-L38</f>
-        <v>1.3200000000000216</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2197,18 +2120,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+      <selection activeCell="A31" sqref="A31:U49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2231,7 +2154,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2269,7 +2192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -2307,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1.68</v>
       </c>
@@ -2345,7 +2268,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2.2400000000000002</v>
       </c>
@@ -2383,7 +2306,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.4</v>
       </c>
@@ -2421,7 +2344,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2.2400000000000002</v>
       </c>
@@ -2459,7 +2382,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1.68</v>
       </c>
@@ -2497,7 +2420,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1.4</v>
       </c>
@@ -2535,7 +2458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1.68</v>
       </c>
@@ -2573,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>3.08</v>
       </c>
@@ -2611,7 +2534,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2.2400000000000002</v>
       </c>
@@ -2649,7 +2572,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>7.84</v>
       </c>
@@ -2687,7 +2610,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2.8</v>
       </c>
@@ -2725,7 +2648,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>4.4800000000000004</v>
       </c>
@@ -2763,7 +2686,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1.68</v>
       </c>
@@ -2801,7 +2724,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>3.36</v>
       </c>
@@ -2839,7 +2762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1.68</v>
       </c>
@@ -2877,7 +2800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>1.68</v>
       </c>
@@ -2915,7 +2838,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>1.68</v>
       </c>
@@ -2953,7 +2876,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>1.68</v>
       </c>
@@ -2991,7 +2914,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>2.52</v>
       </c>
@@ -3029,7 +2952,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -3052,7 +2975,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -3060,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -3089,15 +3012,15 @@
         <v>83.11999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -3105,9 +3028,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B29">
         <f>B28*B27</f>
@@ -3134,9 +3057,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B31">
         <f>3*2.8</f>
@@ -3154,18 +3077,10 @@
         <f>1*2.8</f>
         <v>2.8</v>
       </c>
-      <c r="J31">
-        <f>1*2.8</f>
-        <v>2.8</v>
-      </c>
-      <c r="L31">
-        <f>1*2.8</f>
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B33">
         <f>B31+B29+B25</f>
@@ -3185,248 +3100,192 @@
       </c>
       <c r="J33">
         <f>J31+J29+J25</f>
-        <v>146.56</v>
+        <v>143.76000000000002</v>
       </c>
       <c r="L33">
         <f>L31+L29+L25</f>
-        <v>145.91999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>16</v>
+        <v>143.12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B34">
-        <f>B33-2</f>
-        <v>150.24</v>
+        <f>B33/2.8</f>
+        <v>54.371428571428581</v>
       </c>
       <c r="D34">
-        <f>D33-2</f>
-        <v>142.07999999999998</v>
+        <f>D33/2.8</f>
+        <v>51.457142857142856</v>
       </c>
       <c r="F34">
-        <f>F33-2</f>
-        <v>143.84</v>
+        <f>F33/2.8</f>
+        <v>52.085714285714289</v>
       </c>
       <c r="H34">
-        <f>H33-2</f>
-        <v>144.44</v>
+        <f>H33/2.8</f>
+        <v>52.300000000000004</v>
       </c>
       <c r="J34">
-        <f>J33-2</f>
-        <v>144.56</v>
+        <f>J33/2.8</f>
+        <v>51.342857142857156</v>
       </c>
       <c r="L34">
-        <f>L33-2</f>
-        <v>143.91999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+        <f>L33/2.8</f>
+        <v>51.114285714285721</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35">
-        <f>B34/2.8</f>
-        <v>53.657142857142865</v>
-      </c>
-      <c r="D35">
-        <f t="shared" ref="D35:L35" si="0">D34/2.8</f>
-        <v>50.74285714285714</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="0"/>
-        <v>51.371428571428574</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="0"/>
-        <v>51.585714285714289</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="0"/>
-        <v>51.628571428571433</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="0"/>
-        <v>51.4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="1">
+        <f>ROUND(B34,0)</f>
+        <v>54</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1">
+        <f>ROUND(D34,0)</f>
+        <v>51</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1">
+        <f>ROUND(F34,0)</f>
+        <v>52</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1">
+        <f>ROUND(H34,0)</f>
+        <v>52</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1">
+        <f>ROUND(J34,0)</f>
+        <v>51</v>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1">
+        <f>ROUND(L34,0)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R36" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="1">
-        <f>ROUND(B35,0)</f>
-        <v>54</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1">
-        <f>ROUND(D35,0)</f>
-        <v>51</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1">
-        <f>ROUND(F35,0)</f>
-        <v>51</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1">
-        <f>ROUND(H35,0)</f>
-        <v>52</v>
-      </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1">
-        <f>ROUND(J35,0)</f>
-        <v>52</v>
-      </c>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1">
-        <f>ROUND(L35,0)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N37" t="s">
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <f>B35*2.8</f>
+        <v>151.19999999999999</v>
+      </c>
+      <c r="D37">
+        <f>D35*2.8</f>
+        <v>142.79999999999998</v>
+      </c>
+      <c r="F37">
+        <f>F35*2.8</f>
+        <v>145.6</v>
+      </c>
+      <c r="H37">
+        <f>H35*2.8</f>
+        <v>145.6</v>
+      </c>
+      <c r="J37">
+        <f>J35*2.8</f>
+        <v>142.79999999999998</v>
+      </c>
+      <c r="L37">
+        <f>L35*2.8</f>
+        <v>142.79999999999998</v>
+      </c>
+      <c r="R37" s="2">
+        <f>(SUM(B37:L37))/60</f>
+        <v>14.513333333333332</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38">
+        <f>B33+7</f>
+        <v>159.24</v>
+      </c>
+      <c r="D38">
+        <f>D33+7</f>
+        <v>151.07999999999998</v>
+      </c>
+      <c r="F38">
+        <f>F33+7</f>
+        <v>152.84</v>
+      </c>
+      <c r="H38">
+        <f>H33+7</f>
+        <v>153.44</v>
+      </c>
+      <c r="J38">
+        <f>J33+7</f>
+        <v>150.76000000000002</v>
+      </c>
+      <c r="L38">
+        <f>L33+7</f>
+        <v>150.12</v>
+      </c>
+      <c r="R38" s="2">
+        <f>(SUM(B38:L38))/60</f>
+        <v>15.291333333333332</v>
+      </c>
+      <c r="S38">
+        <v>7</v>
+      </c>
+      <c r="T38">
+        <v>3</v>
+      </c>
+      <c r="U38" s="1">
+        <f>R38+T38*S38/60</f>
+        <v>15.641333333333332</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39">
+        <f>B38-B37</f>
+        <v>8.0400000000000205</v>
+      </c>
+      <c r="D39">
+        <f>D38-D37</f>
+        <v>8.2800000000000011</v>
+      </c>
+      <c r="F39">
+        <f>F38-F37</f>
+        <v>7.2400000000000091</v>
+      </c>
+      <c r="H39">
+        <f>H38-H37</f>
+        <v>7.8400000000000034</v>
+      </c>
+      <c r="J39">
+        <f>J38-J37</f>
+        <v>7.9600000000000364</v>
+      </c>
+      <c r="L39">
+        <f>L38-L37</f>
+        <v>7.3200000000000216</v>
+      </c>
+      <c r="S39" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38">
-        <f>B36*2.8</f>
-        <v>151.19999999999999</v>
-      </c>
-      <c r="D38">
-        <f>D36*2.8</f>
-        <v>142.79999999999998</v>
-      </c>
-      <c r="F38">
-        <f>F36*2.8</f>
-        <v>142.79999999999998</v>
-      </c>
-      <c r="H38">
-        <f>H36*2.8</f>
-        <v>145.6</v>
-      </c>
-      <c r="J38">
-        <f>J36*2.8</f>
-        <v>145.6</v>
-      </c>
-      <c r="L38">
-        <f>L36*2.8</f>
-        <v>142.79999999999998</v>
-      </c>
-      <c r="N38" s="1">
-        <f>(SUM(B38:L38))/60</f>
-        <v>14.513333333333332</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>18</v>
-      </c>
-      <c r="B39">
-        <f>B31+B29+B25</f>
-        <v>152.24</v>
-      </c>
-      <c r="D39">
-        <f>D31+D29+D25</f>
-        <v>144.07999999999998</v>
-      </c>
-      <c r="F39">
-        <f>F31+F29+F25</f>
-        <v>145.84</v>
-      </c>
-      <c r="H39">
-        <f>H31+H29+H25</f>
-        <v>146.44</v>
-      </c>
-      <c r="J39">
-        <f>J31+J29+J25</f>
-        <v>146.56</v>
-      </c>
-      <c r="L39">
-        <f>L31+L29+L25</f>
-        <v>145.91999999999999</v>
-      </c>
-      <c r="N39" s="1">
-        <f>(SUM(B39:L39))/60</f>
-        <v>14.684666666666663</v>
-      </c>
-      <c r="O39">
-        <v>14</v>
-      </c>
-      <c r="P39">
-        <v>5</v>
-      </c>
-      <c r="Q39" s="1">
-        <f>N39+(O39*P39)/60</f>
-        <v>15.851333333333329</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40">
-        <f>B39-B38</f>
-        <v>1.0400000000000205</v>
-      </c>
-      <c r="D40">
-        <f>D39-D38</f>
-        <v>1.2800000000000011</v>
-      </c>
-      <c r="F40">
-        <f>F39-F38</f>
-        <v>3.0400000000000205</v>
-      </c>
-      <c r="H40">
-        <f>H39-H38</f>
-        <v>0.84000000000000341</v>
-      </c>
-      <c r="J40">
-        <f>J39-J38</f>
-        <v>0.96000000000000796</v>
-      </c>
-      <c r="L40">
-        <f>L39-L38</f>
-        <v>3.1200000000000045</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3439,15 +3298,15 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="Q68" sqref="Q68"/>
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3464,7 +3323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -3490,7 +3349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -3516,7 +3375,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2.2400000000000002</v>
       </c>
@@ -3542,7 +3401,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>6.16</v>
       </c>
@@ -3568,7 +3427,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.1200000000000001</v>
       </c>
@@ -3594,7 +3453,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.84</v>
       </c>
@@ -3620,7 +3479,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1.1200000000000001</v>
       </c>
@@ -3646,7 +3505,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2.2400000000000002</v>
       </c>
@@ -3672,7 +3531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.84</v>
       </c>
@@ -3698,7 +3557,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.56000000000000005</v>
       </c>
@@ -3724,7 +3583,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.84</v>
       </c>
@@ -3750,7 +3609,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2.52</v>
       </c>
@@ -3776,7 +3635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.56000000000000005</v>
       </c>
@@ -3802,7 +3661,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1.68</v>
       </c>
@@ -3828,7 +3687,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.56000000000000005</v>
       </c>
@@ -3854,7 +3713,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.84</v>
       </c>
@@ -3880,7 +3739,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>3.92</v>
       </c>
@@ -3906,7 +3765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0.84</v>
       </c>
@@ -3932,7 +3791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0.56000000000000005</v>
       </c>
@@ -3958,7 +3817,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2.2400000000000002</v>
       </c>
@@ -3984,7 +3843,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>3.92</v>
       </c>
@@ -4010,7 +3869,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>1.68</v>
       </c>
@@ -4036,7 +3895,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>2.52</v>
       </c>
@@ -4062,7 +3921,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>3.64</v>
       </c>
@@ -4088,7 +3947,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>3.08</v>
       </c>
@@ -4114,7 +3973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>0.56000000000000005</v>
       </c>
@@ -4140,7 +3999,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>8.68</v>
       </c>
@@ -4166,7 +4025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0.84</v>
       </c>
@@ -4192,7 +4051,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>0.84</v>
       </c>
@@ -4218,7 +4077,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>0.84</v>
       </c>
@@ -4244,7 +4103,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>1.1200000000000001</v>
       </c>
@@ -4270,7 +4129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>1.1200000000000001</v>
       </c>
@@ -4296,7 +4155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>3.36</v>
       </c>
@@ -4322,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>0.84</v>
       </c>
@@ -4348,7 +4207,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>0.84</v>
       </c>
@@ -4374,7 +4233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>8.1199999999999992</v>
       </c>
@@ -4400,7 +4259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>2.2400000000000002</v>
       </c>
@@ -4426,7 +4285,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>0.84</v>
       </c>
@@ -4452,7 +4311,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>1.96</v>
       </c>
@@ -4478,7 +4337,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.84</v>
       </c>
@@ -4504,7 +4363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>1.1200000000000001</v>
       </c>
@@ -4530,7 +4389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>2.52</v>
       </c>
@@ -4556,7 +4415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>0.84</v>
       </c>
@@ -4582,7 +4441,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>0.84</v>
       </c>
@@ -4608,7 +4467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>0.84</v>
       </c>
@@ -4634,7 +4493,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>1.1200000000000001</v>
       </c>
@@ -4660,7 +4519,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>0.84</v>
       </c>
@@ -4686,7 +4545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>5.04</v>
       </c>
@@ -4712,7 +4571,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>1.1200000000000001</v>
       </c>
@@ -4738,7 +4597,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -4755,7 +4614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -4763,7 +4622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -4784,15 +4643,15 @@
         <v>155.28000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B56">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -4800,9 +4659,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B58">
         <f>B57*B56</f>
@@ -4821,9 +4680,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B60">
         <f>3*2.8</f>
@@ -4842,9 +4701,9 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B62">
         <f>B60+B58+B54</f>
@@ -4863,180 +4722,167 @@
         <v>302.08000000000004</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>16</v>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B63">
-        <f>B62-2</f>
-        <v>307.24000000000007</v>
+        <f>B62/2.8</f>
+        <v>110.44285714285718</v>
       </c>
       <c r="D63">
-        <f>D62-2</f>
-        <v>298.96000000000009</v>
+        <f>D62/2.8</f>
+        <v>107.48571428571432</v>
       </c>
       <c r="F63">
-        <f>F62-2</f>
-        <v>288.88000000000005</v>
+        <f>F62/2.8</f>
+        <v>103.88571428571431</v>
       </c>
       <c r="H63">
-        <f>H62-2</f>
-        <v>300.08000000000004</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+        <f>H62/2.8</f>
+        <v>107.8857142857143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B64">
-        <f>B63/2.8</f>
-        <v>109.72857142857146</v>
-      </c>
-      <c r="D64">
-        <f t="shared" ref="D64:H64" si="0">D63/2.8</f>
-        <v>106.77142857142861</v>
-      </c>
-      <c r="F64">
-        <f t="shared" si="0"/>
-        <v>103.17142857142859</v>
-      </c>
-      <c r="H64">
-        <f t="shared" si="0"/>
-        <v>107.17142857142859</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" s="1">
+        <f>ROUND(B63,0)</f>
+        <v>110</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1">
+        <f>ROUND(D63,0)</f>
+        <v>107</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1">
+        <f>ROUND(F63,0)</f>
+        <v>104</v>
+      </c>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1">
+        <f>ROUND(H63,0)</f>
+        <v>108</v>
+      </c>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N65" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="1">
-        <f>ROUND(B64,0)</f>
-        <v>110</v>
-      </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1">
-        <f>ROUND(D64,0)</f>
-        <v>107</v>
-      </c>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1">
-        <f>ROUND(F64,0)</f>
-        <v>103</v>
-      </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1">
-        <f>ROUND(H64,0)</f>
-        <v>107</v>
-      </c>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N66" t="s">
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66">
+        <f>B64*2.8</f>
+        <v>308</v>
+      </c>
+      <c r="D66">
+        <f>D64*2.8</f>
+        <v>299.59999999999997</v>
+      </c>
+      <c r="F66">
+        <f>F64*2.8</f>
+        <v>291.2</v>
+      </c>
+      <c r="H66">
+        <f>H64*2.8</f>
+        <v>302.39999999999998</v>
+      </c>
+      <c r="N66" s="2">
+        <f>(SUM(B66:L66))/60</f>
+        <v>20.019999999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67">
+        <f>B62+7</f>
+        <v>316.24000000000007</v>
+      </c>
+      <c r="D67">
+        <f>D62+7</f>
+        <v>307.96000000000009</v>
+      </c>
+      <c r="F67">
+        <f>F62+7</f>
+        <v>297.88000000000005</v>
+      </c>
+      <c r="H67">
+        <f>H62+7</f>
+        <v>309.08000000000004</v>
+      </c>
+      <c r="N67" s="2">
+        <f>(SUM(B67:L67))/60</f>
+        <v>20.519333333333339</v>
+      </c>
+      <c r="O67">
+        <v>7</v>
+      </c>
+      <c r="P67">
+        <v>3</v>
+      </c>
+      <c r="Q67" s="1">
+        <f>N67+P67*O67/60</f>
+        <v>20.869333333333341</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68">
+        <f>B67-B66</f>
+        <v>8.2400000000000659</v>
+      </c>
+      <c r="D68">
+        <f>D67-D66</f>
+        <v>8.3600000000001273</v>
+      </c>
+      <c r="F68">
+        <f>F67-F66</f>
+        <v>6.6800000000000637</v>
+      </c>
+      <c r="H68">
+        <f>H67-H66</f>
+        <v>6.6800000000000637</v>
+      </c>
+      <c r="O68" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>17</v>
-      </c>
-      <c r="B67">
-        <f>B65*2.8</f>
-        <v>308</v>
-      </c>
-      <c r="D67">
-        <f>D65*2.8</f>
-        <v>299.59999999999997</v>
-      </c>
-      <c r="F67">
-        <f>F65*2.8</f>
-        <v>288.39999999999998</v>
-      </c>
-      <c r="H67">
-        <f>H65*2.8</f>
-        <v>299.59999999999997</v>
-      </c>
-      <c r="N67" s="1">
-        <f>(SUM(B67:L67))/60</f>
-        <v>19.926666666666666</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>18</v>
       </c>
-      <c r="B68">
-        <f>B60+B58+B54</f>
-        <v>309.24000000000007</v>
-      </c>
-      <c r="D68">
-        <f>D60+D58+D54</f>
-        <v>300.96000000000009</v>
-      </c>
-      <c r="F68">
-        <f>F60+F58+F54</f>
-        <v>290.88000000000005</v>
-      </c>
-      <c r="H68">
-        <f>H60+H58+H54</f>
-        <v>302.08000000000004</v>
-      </c>
-      <c r="N68" s="1">
-        <f>(SUM(B68:L68))/60</f>
-        <v>20.052666666666671</v>
-      </c>
-      <c r="O68">
-        <v>14</v>
-      </c>
-      <c r="P68">
-        <v>3</v>
-      </c>
-      <c r="Q68" s="1">
-        <f>N68+(O68*P68)/60</f>
-        <v>20.75266666666667</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>20</v>
       </c>
-      <c r="B69">
-        <f>B68-B67</f>
-        <v>1.2400000000000659</v>
-      </c>
-      <c r="D69">
-        <f>D68-D67</f>
-        <v>1.3600000000001273</v>
-      </c>
-      <c r="F69">
-        <f>F68-F67</f>
-        <v>2.480000000000075</v>
-      </c>
-      <c r="H69">
-        <f>H68-H67</f>
-        <v>2.480000000000075</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -5046,18 +4892,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="Q68" sqref="O68:Q68"/>
+      <selection activeCell="Q71" sqref="A60:Q71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5074,7 +4920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -5100,7 +4946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -5126,7 +4972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1.4</v>
       </c>
@@ -5152,7 +4998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1.68</v>
       </c>
@@ -5178,7 +5024,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0.84</v>
       </c>
@@ -5204,7 +5050,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2.52</v>
       </c>
@@ -5230,7 +5076,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.84</v>
       </c>
@@ -5256,7 +5102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1.4</v>
       </c>
@@ -5282,7 +5128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1.68</v>
       </c>
@@ -5308,7 +5154,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>3.92</v>
       </c>
@@ -5334,7 +5180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.84</v>
       </c>
@@ -5360,7 +5206,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.84</v>
       </c>
@@ -5386,7 +5232,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.56000000000000005</v>
       </c>
@@ -5412,7 +5258,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1.96</v>
       </c>
@@ -5438,7 +5284,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.84</v>
       </c>
@@ -5464,7 +5310,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2.8</v>
       </c>
@@ -5490,7 +5336,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>3.36</v>
       </c>
@@ -5516,7 +5362,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>3.08</v>
       </c>
@@ -5542,7 +5388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0.56000000000000005</v>
       </c>
@@ -5568,7 +5414,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>1.96</v>
       </c>
@@ -5594,7 +5440,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>1.96</v>
       </c>
@@ -5620,7 +5466,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>1.96</v>
       </c>
@@ -5646,7 +5492,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1.1200000000000001</v>
       </c>
@@ -5672,7 +5518,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>1.1200000000000001</v>
       </c>
@@ -5698,7 +5544,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>3.92</v>
       </c>
@@ -5724,7 +5570,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>3.64</v>
       </c>
@@ -5750,7 +5596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>1.68</v>
       </c>
@@ -5776,7 +5622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>2.2400000000000002</v>
       </c>
@@ -5802,7 +5648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>0.56000000000000005</v>
       </c>
@@ -5828,7 +5674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>5.88</v>
       </c>
@@ -5854,7 +5700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>1.68</v>
       </c>
@@ -5880,7 +5726,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>1.4</v>
       </c>
@@ -5906,7 +5752,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>1.4</v>
       </c>
@@ -5932,7 +5778,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>0.84</v>
       </c>
@@ -5958,7 +5804,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>1.1200000000000001</v>
       </c>
@@ -5984,7 +5830,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>1.1200000000000001</v>
       </c>
@@ -6010,7 +5856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>1.1200000000000001</v>
       </c>
@@ -6036,7 +5882,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>5.88</v>
       </c>
@@ -6062,7 +5908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>1.4</v>
       </c>
@@ -6088,7 +5934,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.84</v>
       </c>
@@ -6114,7 +5960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>1.4</v>
       </c>
@@ -6140,7 +5986,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>0.84</v>
       </c>
@@ -6166,7 +6012,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>1.68</v>
       </c>
@@ -6192,7 +6038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>2.2400000000000002</v>
       </c>
@@ -6218,7 +6064,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>0.56000000000000005</v>
       </c>
@@ -6244,7 +6090,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>3.08</v>
       </c>
@@ -6270,7 +6116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>1.68</v>
       </c>
@@ -6296,7 +6142,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>0.56000000000000005</v>
       </c>
@@ -6322,7 +6168,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>1.1200000000000001</v>
       </c>
@@ -6348,7 +6194,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -6365,7 +6211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -6373,7 +6219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -6394,15 +6240,15 @@
         <v>154.44000000000008</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B56">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -6410,9 +6256,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B58">
         <f>B57*B56</f>
@@ -6431,9 +6277,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B60">
         <f>3*2.8</f>
@@ -6452,9 +6298,9 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B62">
         <f>B60+B58+B54</f>
@@ -6473,180 +6319,152 @@
         <v>301.24000000000012</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>16</v>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B63">
-        <f>B62-2</f>
-        <v>300.52000000000004</v>
+        <f>B62/2.8</f>
+        <v>108.04285714285716</v>
       </c>
       <c r="D63">
-        <f>D62-2</f>
-        <v>299.24000000000007</v>
+        <f>D62/2.8</f>
+        <v>107.58571428571432</v>
       </c>
       <c r="F63">
-        <f>F62-2</f>
-        <v>286.64000000000004</v>
+        <f>F62/2.8</f>
+        <v>103.0857142857143</v>
       </c>
       <c r="H63">
-        <f>H62-2</f>
-        <v>299.24000000000012</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+        <f>H62/2.8</f>
+        <v>107.58571428571433</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B64">
-        <f>B63/2.8</f>
-        <v>107.32857142857145</v>
-      </c>
-      <c r="D64">
-        <f t="shared" ref="D64:H64" si="0">D63/2.8</f>
-        <v>106.87142857142859</v>
-      </c>
-      <c r="F64">
-        <f t="shared" si="0"/>
-        <v>102.37142857142859</v>
-      </c>
-      <c r="H64">
-        <f t="shared" si="0"/>
-        <v>106.87142857142862</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" s="1">
+        <f>ROUND(B63,0)</f>
+        <v>108</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1">
+        <f>ROUND(D63,0)</f>
+        <v>108</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1">
+        <f>ROUND(F63,0)</f>
+        <v>103</v>
+      </c>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1">
+        <f>ROUND(H63,0)</f>
+        <v>108</v>
+      </c>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N65" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="1">
-        <f>ROUND(B64,0)</f>
-        <v>107</v>
-      </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1">
-        <f>ROUND(D64,0)</f>
-        <v>107</v>
-      </c>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1">
-        <f>ROUND(F64,0)</f>
-        <v>102</v>
-      </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1">
-        <f>ROUND(H64,0)</f>
-        <v>107</v>
-      </c>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N66" t="s">
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66">
+        <f>B64*2.8</f>
+        <v>302.39999999999998</v>
+      </c>
+      <c r="D66">
+        <f>D64*2.8</f>
+        <v>302.39999999999998</v>
+      </c>
+      <c r="F66">
+        <f>F64*2.8</f>
+        <v>288.39999999999998</v>
+      </c>
+      <c r="H66">
+        <f>H64*2.8</f>
+        <v>302.39999999999998</v>
+      </c>
+      <c r="N66" s="2">
+        <f>(SUM(B66:L66))/60</f>
+        <v>19.926666666666666</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67">
+        <f>B62+7</f>
+        <v>309.52000000000004</v>
+      </c>
+      <c r="D67">
+        <f>D62+7</f>
+        <v>308.24000000000007</v>
+      </c>
+      <c r="F67">
+        <f>F62+7</f>
+        <v>295.64000000000004</v>
+      </c>
+      <c r="H67">
+        <f>H62+7</f>
+        <v>308.24000000000012</v>
+      </c>
+      <c r="N67" s="2">
+        <f>(SUM(B67:L67))/60</f>
+        <v>20.36066666666667</v>
+      </c>
+      <c r="O67">
+        <v>7</v>
+      </c>
+      <c r="P67">
+        <v>3</v>
+      </c>
+      <c r="Q67" s="1">
+        <f>N67+P67*O67/60</f>
+        <v>20.710666666666672</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68">
+        <f>B67-B66</f>
+        <v>7.1200000000000614</v>
+      </c>
+      <c r="D68">
+        <f>D67-D66</f>
+        <v>5.8400000000000887</v>
+      </c>
+      <c r="F68">
+        <f>F67-F66</f>
+        <v>7.2400000000000659</v>
+      </c>
+      <c r="H68">
+        <f>H67-H66</f>
+        <v>5.8400000000001455</v>
+      </c>
+      <c r="O68" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>17</v>
-      </c>
-      <c r="B67">
-        <f>B65*2.8</f>
-        <v>299.59999999999997</v>
-      </c>
-      <c r="D67">
-        <f>D65*2.8</f>
-        <v>299.59999999999997</v>
-      </c>
-      <c r="F67">
-        <f>F65*2.8</f>
-        <v>285.59999999999997</v>
-      </c>
-      <c r="H67">
-        <f>H65*2.8</f>
-        <v>299.59999999999997</v>
-      </c>
-      <c r="N67" s="1">
-        <f>(SUM(B67:L67))/60</f>
-        <v>19.739999999999998</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>18</v>
       </c>
-      <c r="B68">
-        <f>B60+B58+B54</f>
-        <v>302.52000000000004</v>
-      </c>
-      <c r="D68">
-        <f>D60+D58+D54</f>
-        <v>301.24000000000007</v>
-      </c>
-      <c r="F68">
-        <f>F60+F58+F54</f>
-        <v>288.64000000000004</v>
-      </c>
-      <c r="H68">
-        <f>H60+H58+H54</f>
-        <v>301.24000000000012</v>
-      </c>
-      <c r="N68" s="1">
-        <f>(SUM(B68:L68))/60</f>
-        <v>19.894000000000005</v>
-      </c>
-      <c r="O68">
-        <v>14</v>
-      </c>
-      <c r="P68">
-        <v>3</v>
-      </c>
-      <c r="Q68" s="1">
-        <f>N68+(O68*P68)/60</f>
-        <v>20.594000000000005</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>20</v>
-      </c>
-      <c r="B69">
-        <f>B68-B67</f>
-        <v>2.9200000000000728</v>
-      </c>
-      <c r="D69">
-        <f>D68-D67</f>
-        <v>1.6400000000001</v>
-      </c>
-      <c r="F69">
-        <f>F68-F67</f>
-        <v>3.0400000000000773</v>
-      </c>
-      <c r="H69">
-        <f>H68-H67</f>
-        <v>1.6400000000001569</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -6656,18 +6474,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="Q52" sqref="O52:Q52"/>
+      <selection activeCell="Q55" sqref="A44:Q55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6684,7 +6502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -6710,7 +6528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -6736,7 +6554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.56000000000000005</v>
       </c>
@@ -6762,7 +6580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2.52</v>
       </c>
@@ -6788,7 +6606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.4</v>
       </c>
@@ -6814,7 +6632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1.96</v>
       </c>
@@ -6840,7 +6658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1.1200000000000001</v>
       </c>
@@ -6866,7 +6684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1.68</v>
       </c>
@@ -6892,7 +6710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1.1200000000000001</v>
       </c>
@@ -6918,7 +6736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>1.4</v>
       </c>
@@ -6944,7 +6762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1.4</v>
       </c>
@@ -6970,7 +6788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1.96</v>
       </c>
@@ -6996,7 +6814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.56000000000000005</v>
       </c>
@@ -7022,7 +6840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2.8</v>
       </c>
@@ -7048,7 +6866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>3.64</v>
       </c>
@@ -7074,7 +6892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.56000000000000005</v>
       </c>
@@ -7100,7 +6918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1.1200000000000001</v>
       </c>
@@ -7126,7 +6944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2.52</v>
       </c>
@@ -7152,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0.84</v>
       </c>
@@ -7178,7 +6996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0.84</v>
       </c>
@@ -7204,7 +7022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>1.68</v>
       </c>
@@ -7230,7 +7048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0.56000000000000005</v>
       </c>
@@ -7256,7 +7074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>0.56000000000000005</v>
       </c>
@@ -7282,7 +7100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>1.68</v>
       </c>
@@ -7308,7 +7126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0.84</v>
       </c>
@@ -7334,7 +7152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>3.08</v>
       </c>
@@ -7360,7 +7178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>1.96</v>
       </c>
@@ -7386,7 +7204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>4.76</v>
       </c>
@@ -7412,7 +7230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>2.2400000000000002</v>
       </c>
@@ -7438,7 +7256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>1.68</v>
       </c>
@@ -7464,7 +7282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.84</v>
       </c>
@@ -7490,7 +7308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0.84</v>
       </c>
@@ -7516,7 +7334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>1.4</v>
       </c>
@@ -7542,7 +7360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -7559,7 +7377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -7567,7 +7385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -7588,15 +7406,15 @@
         <v>108.48000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B40">
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -7604,9 +7422,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B42">
         <f>B41*B40</f>
@@ -7625,9 +7443,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B44">
         <f>3*2.8</f>
@@ -7646,9 +7464,9 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B46">
         <f>B44+B42+B38</f>
@@ -7667,180 +7485,152 @@
         <v>159.28000000000003</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>16</v>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B47">
-        <f>B46-2</f>
-        <v>153.52000000000004</v>
+        <f>B46/2.8</f>
+        <v>55.542857142857159</v>
       </c>
       <c r="D47">
-        <f>D46-2</f>
-        <v>156.44000000000003</v>
+        <f>D46/2.8</f>
+        <v>56.585714285714296</v>
       </c>
       <c r="F47">
-        <f>F46-2</f>
-        <v>158.12</v>
+        <f>F46/2.8</f>
+        <v>57.18571428571429</v>
       </c>
       <c r="H47">
-        <f>H46-2</f>
-        <v>157.28000000000003</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <f>H46/2.8</f>
+        <v>56.8857142857143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48">
-        <f>B47/2.8</f>
-        <v>54.828571428571443</v>
-      </c>
-      <c r="D48">
-        <f t="shared" ref="D48:H48" si="0">D47/2.8</f>
-        <v>55.871428571428581</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="0"/>
-        <v>56.471428571428575</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="0"/>
-        <v>56.171428571428585</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="1">
+        <f>ROUND(B47,0)</f>
+        <v>56</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1">
+        <f>ROUND(D47,0)</f>
+        <v>57</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1">
+        <f>ROUND(F47,0)</f>
+        <v>57</v>
+      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1">
+        <f>ROUND(H47,0)</f>
+        <v>57</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="1">
-        <f>ROUND(B48,0)</f>
-        <v>55</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1">
-        <f>ROUND(D48,0)</f>
-        <v>56</v>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1">
-        <f>ROUND(F48,0)</f>
-        <v>56</v>
-      </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1">
-        <f>ROUND(H48,0)</f>
-        <v>56</v>
-      </c>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50">
+        <f>B48*2.8</f>
+        <v>156.79999999999998</v>
+      </c>
+      <c r="D50">
+        <f>D48*2.8</f>
+        <v>159.6</v>
+      </c>
+      <c r="F50">
+        <f>F48*2.8</f>
+        <v>159.6</v>
+      </c>
+      <c r="H50">
+        <f>H48*2.8</f>
+        <v>159.6</v>
+      </c>
+      <c r="N50" s="1">
+        <f>(SUM(B50:L50))/60</f>
+        <v>10.593333333333334</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B51">
-        <f>B49*2.8</f>
-        <v>154</v>
+        <f>B46+7</f>
+        <v>162.52000000000004</v>
       </c>
       <c r="D51">
-        <f>D49*2.8</f>
-        <v>156.79999999999998</v>
+        <f>D46+7</f>
+        <v>165.44000000000003</v>
       </c>
       <c r="F51">
-        <f>F49*2.8</f>
-        <v>156.79999999999998</v>
+        <f>F46+7</f>
+        <v>167.12</v>
       </c>
       <c r="H51">
-        <f>H49*2.8</f>
-        <v>156.79999999999998</v>
+        <f>H46+7</f>
+        <v>166.28000000000003</v>
       </c>
       <c r="N51" s="1">
         <f>(SUM(B51:L51))/60</f>
-        <v>10.406666666666665</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+        <v>11.022666666666669</v>
+      </c>
+      <c r="O51">
+        <v>7</v>
+      </c>
+      <c r="P51">
+        <v>3</v>
+      </c>
+      <c r="Q51" s="1">
+        <f>N51+P51*O51/60</f>
+        <v>11.372666666666669</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52">
+        <f>B51-B50</f>
+        <v>5.7200000000000557</v>
+      </c>
+      <c r="D52">
+        <f>D51-D50</f>
+        <v>5.8400000000000318</v>
+      </c>
+      <c r="F52">
+        <f>F51-F50</f>
+        <v>7.5200000000000102</v>
+      </c>
+      <c r="H52">
+        <f>H51-H50</f>
+        <v>6.6800000000000352</v>
+      </c>
+      <c r="O52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>18</v>
       </c>
-      <c r="B52">
-        <f>B44+B42+B38</f>
-        <v>155.52000000000004</v>
-      </c>
-      <c r="D52">
-        <f>D44+D42+D38</f>
-        <v>158.44000000000003</v>
-      </c>
-      <c r="F52">
-        <f>F44+F42+F38</f>
-        <v>160.12</v>
-      </c>
-      <c r="H52">
-        <f>H44+H42+H38</f>
-        <v>159.28000000000003</v>
-      </c>
-      <c r="N52" s="1">
-        <f>(SUM(B52:L52))/60</f>
-        <v>10.556000000000003</v>
-      </c>
-      <c r="O52">
-        <v>14</v>
-      </c>
-      <c r="P52">
-        <v>3</v>
-      </c>
-      <c r="Q52" s="1">
-        <f>N52+(O52*P52)/60</f>
-        <v>11.256000000000002</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>20</v>
-      </c>
-      <c r="B53">
-        <f>B52-B51</f>
-        <v>1.5200000000000387</v>
-      </c>
-      <c r="D53">
-        <f>D52-D51</f>
-        <v>1.6400000000000432</v>
-      </c>
-      <c r="F53">
-        <f>F52-F51</f>
-        <v>3.3200000000000216</v>
-      </c>
-      <c r="H53">
-        <f>H52-H51</f>
-        <v>2.4800000000000466</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B57" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B58" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -7850,18 +7640,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="Q56" sqref="A44:Q56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7878,7 +7668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -7904,7 +7694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -7930,7 +7720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.84</v>
       </c>
@@ -7956,7 +7746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0.84</v>
       </c>
@@ -7982,7 +7772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>7.28</v>
       </c>
@@ -8008,7 +7798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2.52</v>
       </c>
@@ -8034,7 +7824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1.1200000000000001</v>
       </c>
@@ -8060,7 +7850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1.96</v>
       </c>
@@ -8086,7 +7876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.84</v>
       </c>
@@ -8112,7 +7902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.84</v>
       </c>
@@ -8138,7 +7928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.84</v>
       </c>
@@ -8164,7 +7954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.56000000000000005</v>
       </c>
@@ -8190,7 +7980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1.68</v>
       </c>
@@ -8216,7 +8006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1.68</v>
       </c>
@@ -8242,7 +8032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.84</v>
       </c>
@@ -8268,7 +8058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.84</v>
       </c>
@@ -8294,7 +8084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1.68</v>
       </c>
@@ -8320,7 +8110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0.84</v>
       </c>
@@ -8346,7 +8136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0.56000000000000005</v>
       </c>
@@ -8372,7 +8162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0.84</v>
       </c>
@@ -8398,7 +8188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.84</v>
       </c>
@@ -8424,7 +8214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>6.72</v>
       </c>
@@ -8450,7 +8240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>5.88</v>
       </c>
@@ -8476,7 +8266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>1.1200000000000001</v>
       </c>
@@ -8502,7 +8292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>1.1200000000000001</v>
       </c>
@@ -8528,7 +8318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>1.1200000000000001</v>
       </c>
@@ -8554,7 +8344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>4.76</v>
       </c>
@@ -8580,7 +8370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>1.68</v>
       </c>
@@ -8606,7 +8396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>3.36</v>
       </c>
@@ -8632,7 +8422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>3.92</v>
       </c>
@@ -8658,7 +8448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.84</v>
       </c>
@@ -8684,7 +8474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>1.1200000000000001</v>
       </c>
@@ -8710,7 +8500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>0.56000000000000005</v>
       </c>
@@ -8736,7 +8526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -8753,7 +8543,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -8761,7 +8551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -8782,15 +8572,15 @@
         <v>99.240000000000038</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B40">
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -8798,9 +8588,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B42">
         <f>B41*B40</f>
@@ -8819,9 +8609,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B44">
         <f>3*2.8</f>
@@ -8840,9 +8630,9 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B46">
         <f>B44+B42+B38</f>
@@ -8861,180 +8651,152 @@
         <v>150.04000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>16</v>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B47">
-        <f>B46-2</f>
-        <v>163.04000000000005</v>
+        <f>B46/2.8</f>
+        <v>58.942857142857164</v>
       </c>
       <c r="D47">
-        <f>D46-2</f>
-        <v>153.92000000000002</v>
+        <f>D46/2.8</f>
+        <v>55.685714285714297</v>
       </c>
       <c r="F47">
-        <f>F46-2</f>
-        <v>157.56000000000003</v>
+        <f>F46/2.8</f>
+        <v>56.985714285714302</v>
       </c>
       <c r="H47">
-        <f>H46-2</f>
-        <v>148.04000000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <f>H46/2.8</f>
+        <v>53.585714285714296</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48">
-        <f>B47/2.8</f>
-        <v>58.228571428571449</v>
-      </c>
-      <c r="D48">
-        <f t="shared" ref="D48:H48" si="0">D47/2.8</f>
-        <v>54.971428571428582</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="0"/>
-        <v>56.271428571428586</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="0"/>
-        <v>52.871428571428581</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="1">
+        <f>ROUND(B47,0)</f>
+        <v>59</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1">
+        <f>ROUND(D47,0)</f>
+        <v>56</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1">
+        <f>ROUND(F47,0)</f>
+        <v>57</v>
+      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1">
+        <f>ROUND(H47,0)</f>
+        <v>54</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="1">
-        <f>ROUND(B48,0)</f>
-        <v>58</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1">
-        <f>ROUND(D48,0)</f>
-        <v>55</v>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1">
-        <f>ROUND(F48,0)</f>
-        <v>56</v>
-      </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1">
-        <f>ROUND(H48,0)</f>
-        <v>53</v>
-      </c>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50">
+        <f>B48*2.8</f>
+        <v>165.2</v>
+      </c>
+      <c r="D50">
+        <f>D48*2.8</f>
+        <v>156.79999999999998</v>
+      </c>
+      <c r="F50">
+        <f>F48*2.8</f>
+        <v>159.6</v>
+      </c>
+      <c r="H50">
+        <f>H48*2.8</f>
+        <v>151.19999999999999</v>
+      </c>
+      <c r="N50" s="1">
+        <f>(SUM(B50:L50))/60</f>
+        <v>10.546666666666665</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B51">
-        <f>B49*2.8</f>
-        <v>162.39999999999998</v>
+        <f>B46+7</f>
+        <v>172.04000000000005</v>
       </c>
       <c r="D51">
-        <f>D49*2.8</f>
-        <v>154</v>
+        <f>D46+7</f>
+        <v>162.92000000000002</v>
       </c>
       <c r="F51">
-        <f>F49*2.8</f>
-        <v>156.79999999999998</v>
+        <f>F46+7</f>
+        <v>166.56000000000003</v>
       </c>
       <c r="H51">
-        <f>H49*2.8</f>
-        <v>148.39999999999998</v>
+        <f>H46+7</f>
+        <v>157.04000000000002</v>
       </c>
       <c r="N51" s="1">
         <f>(SUM(B51:L51))/60</f>
-        <v>10.359999999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+        <v>10.976000000000003</v>
+      </c>
+      <c r="O51">
+        <v>7</v>
+      </c>
+      <c r="P51">
+        <v>3</v>
+      </c>
+      <c r="Q51" s="1">
+        <f>N51+P51*O51/60</f>
+        <v>11.326000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52">
+        <f>B51-B50</f>
+        <v>6.8400000000000603</v>
+      </c>
+      <c r="D52">
+        <f>D51-D50</f>
+        <v>6.120000000000033</v>
+      </c>
+      <c r="F52">
+        <f>F51-F50</f>
+        <v>6.9600000000000364</v>
+      </c>
+      <c r="H52">
+        <f>H51-H50</f>
+        <v>5.8400000000000318</v>
+      </c>
+      <c r="O52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>18</v>
       </c>
-      <c r="B52">
-        <f>B44+B42+B38</f>
-        <v>165.04000000000005</v>
-      </c>
-      <c r="D52">
-        <f>D44+D42+D38</f>
-        <v>155.92000000000002</v>
-      </c>
-      <c r="F52">
-        <f>F44+F42+F38</f>
-        <v>159.56000000000003</v>
-      </c>
-      <c r="H52">
-        <f>H44+H42+H38</f>
-        <v>150.04000000000002</v>
-      </c>
-      <c r="N52" s="1">
-        <f>(SUM(B52:L52))/60</f>
-        <v>10.509333333333336</v>
-      </c>
-      <c r="O52">
-        <v>14</v>
-      </c>
-      <c r="P52">
-        <v>3</v>
-      </c>
-      <c r="Q52" s="1">
-        <f>N52+(O52*P52)/60</f>
-        <v>11.209333333333335</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>20</v>
-      </c>
-      <c r="B53">
-        <f>B52-B51</f>
-        <v>2.6400000000000716</v>
-      </c>
-      <c r="D53">
-        <f>D52-D51</f>
-        <v>1.9200000000000159</v>
-      </c>
-      <c r="F53">
-        <f>F52-F51</f>
-        <v>2.7600000000000477</v>
-      </c>
-      <c r="H53">
-        <f>H52-H51</f>
-        <v>1.6400000000000432</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B57" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B58" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>